<commit_message>
adds missing concept dpv:ConsentReceipt
- concept was 'lost' due to a regression in the way statuses are tracked
  across versions
- explicitly added the concept in TOMs
- Regression/error will not repeat in the future as we have a stable way
  of working on different versions e.g. 2.0 is this and 2.1-dev is next
</commit_message>
<xml_diff>
--- a/code/vocab_csv/toms.xlsx
+++ b/code/vocab_csv/toms.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="872">
   <si>
     <t>Term</t>
   </si>
@@ -2059,6 +2059,18 @@
   </si>
   <si>
     <t>dpv:DataProcessingRecord</t>
+  </si>
+  <si>
+    <t>ConsentReceipt</t>
+  </si>
+  <si>
+    <t>Consent Receipt</t>
+  </si>
+  <si>
+    <t>A record of consent or consent related activities that is provided to another entity</t>
+  </si>
+  <si>
+    <t>dpv:ConsentRecord</t>
   </si>
   <si>
     <t>ROPA</t>
@@ -20152,7 +20164,7 @@
         <v>558</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>58</v>
@@ -20160,24 +20172,20 @@
       <c r="F66" s="19"/>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
-      <c r="I66" s="31" t="s">
-        <v>559</v>
-      </c>
+      <c r="I66" s="49"/>
       <c r="J66" s="19"/>
       <c r="K66" s="20">
-        <v>44447.0</v>
-      </c>
-      <c r="L66" s="20">
-        <v>45396.0</v>
-      </c>
+        <v>44734.0</v>
+      </c>
+      <c r="L66" s="20"/>
       <c r="M66" s="17" t="s">
         <v>20</v>
       </c>
       <c r="N66" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="O66" s="31" t="s">
-        <v>347</v>
+        <v>53</v>
+      </c>
+      <c r="O66" s="27" t="s">
+        <v>77</v>
       </c>
       <c r="P66" s="19"/>
       <c r="Q66" s="19"/>
@@ -20208,7 +20216,7 @@
         <v>562</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>97</v>
+        <v>555</v>
       </c>
       <c r="E67" s="17" t="s">
         <v>58</v>
@@ -20216,19 +20224,25 @@
       <c r="F67" s="19"/>
       <c r="G67" s="19"/>
       <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="40">
+      <c r="I67" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="J67" s="19"/>
+      <c r="K67" s="20">
+        <v>44447.0</v>
+      </c>
+      <c r="L67" s="20">
         <v>45396.0</v>
       </c>
-      <c r="L67" s="20"/>
       <c r="M67" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N67" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="O67" s="17"/>
+      <c r="N67" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="O67" s="31" t="s">
+        <v>347</v>
+      </c>
       <c r="P67" s="19"/>
       <c r="Q67" s="19"/>
       <c r="R67" s="19"/>
@@ -20249,13 +20263,13 @@
     </row>
     <row r="68">
       <c r="A68" s="17" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D68" s="17" t="s">
         <v>97</v>
@@ -20299,16 +20313,16 @@
     </row>
     <row r="69">
       <c r="A69" s="17" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>555</v>
+        <v>97</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>58</v>
@@ -20348,80 +20362,78 @@
       <c r="AF69" s="19"/>
     </row>
     <row r="70">
-      <c r="A70" s="8"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="17"/>
-      <c r="E70" s="17"/>
+      <c r="A70" s="17" t="s">
+        <v>570</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>572</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>555</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F70" s="19"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="19"/>
+      <c r="I70" s="19"/>
       <c r="J70" s="17"/>
-      <c r="K70" s="40"/>
+      <c r="K70" s="40">
+        <v>45396.0</v>
+      </c>
       <c r="L70" s="20"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="28"/>
+      <c r="M70" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N70" s="28" t="s">
+        <v>53</v>
+      </c>
       <c r="O70" s="17"/>
+      <c r="P70" s="19"/>
+      <c r="Q70" s="19"/>
+      <c r="R70" s="19"/>
+      <c r="S70" s="19"/>
+      <c r="T70" s="19"/>
+      <c r="U70" s="19"/>
+      <c r="V70" s="19"/>
+      <c r="W70" s="19"/>
+      <c r="X70" s="19"/>
+      <c r="Y70" s="19"/>
+      <c r="Z70" s="19"/>
+      <c r="AA70" s="19"/>
+      <c r="AB70" s="19"/>
+      <c r="AC70" s="19"/>
+      <c r="AD70" s="19"/>
+      <c r="AE70" s="19"/>
+      <c r="AF70" s="19"/>
     </row>
     <row r="71">
-      <c r="A71" s="8" t="s">
-        <v>569</v>
-      </c>
-      <c r="B71" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>570</v>
-      </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F71" s="19"/>
-      <c r="G71" s="19"/>
-      <c r="H71" s="19"/>
-      <c r="I71" s="19"/>
+      <c r="A71" s="8"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="17"/>
+      <c r="E71" s="17"/>
       <c r="J71" s="17"/>
-      <c r="K71" s="40">
-        <v>44139.0</v>
-      </c>
+      <c r="K71" s="40"/>
       <c r="L71" s="20"/>
-      <c r="M71" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="N71" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="O71" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="P71" s="19"/>
-      <c r="Q71" s="19"/>
-      <c r="R71" s="19"/>
-      <c r="S71" s="19"/>
-      <c r="T71" s="19"/>
-      <c r="U71" s="19"/>
-      <c r="V71" s="19"/>
-      <c r="W71" s="19"/>
-      <c r="X71" s="19"/>
-      <c r="Y71" s="19"/>
-      <c r="Z71" s="19"/>
-      <c r="AA71" s="19"/>
-      <c r="AB71" s="19"/>
-      <c r="AC71" s="19"/>
-      <c r="AD71" s="19"/>
-      <c r="AE71" s="19"/>
-      <c r="AF71" s="19"/>
+      <c r="M71" s="17"/>
+      <c r="N71" s="28"/>
+      <c r="O71" s="17"/>
     </row>
     <row r="72">
-      <c r="A72" s="17" t="s">
-        <v>571</v>
+      <c r="A72" s="8" t="s">
+        <v>573</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>573</v>
-      </c>
-      <c r="D72" s="17" t="s">
         <v>574</v>
       </c>
+      <c r="D72" s="19"/>
       <c r="E72" s="17" t="s">
         <v>58</v>
       </c>
@@ -20434,7 +20446,7 @@
         <v>44139.0</v>
       </c>
       <c r="L72" s="20"/>
-      <c r="M72" s="19" t="s">
+      <c r="M72" s="17" t="s">
         <v>20</v>
       </c>
       <c r="N72" s="28" t="s">
@@ -20468,11 +20480,11 @@
       <c r="B73" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="C73" s="72" t="s">
+      <c r="C73" s="17" t="s">
         <v>577</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>58</v>
@@ -20482,18 +20494,18 @@
       <c r="H73" s="19"/>
       <c r="I73" s="19"/>
       <c r="J73" s="17"/>
-      <c r="K73" s="20">
-        <v>44727.0</v>
+      <c r="K73" s="40">
+        <v>44139.0</v>
       </c>
       <c r="L73" s="20"/>
-      <c r="M73" s="17" t="s">
+      <c r="M73" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="N73" s="17" t="s">
-        <v>359</v>
-      </c>
-      <c r="O73" s="21" t="s">
-        <v>212</v>
+      <c r="N73" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="O73" s="27" t="s">
+        <v>200</v>
       </c>
       <c r="P73" s="19"/>
       <c r="Q73" s="19"/>
@@ -20515,16 +20527,16 @@
     </row>
     <row r="74">
       <c r="A74" s="17" t="s">
+        <v>579</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="C74" s="72" t="s">
+        <v>581</v>
+      </c>
+      <c r="D74" s="17" t="s">
         <v>578</v>
-      </c>
-      <c r="B74" s="22" t="s">
-        <v>579</v>
-      </c>
-      <c r="C74" s="72" t="s">
-        <v>580</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>581</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>58</v>
@@ -20535,7 +20547,7 @@
       <c r="I74" s="19"/>
       <c r="J74" s="17"/>
       <c r="K74" s="20">
-        <v>44856.0</v>
+        <v>44727.0</v>
       </c>
       <c r="L74" s="20"/>
       <c r="M74" s="17" t="s">
@@ -20544,7 +20556,9 @@
       <c r="N74" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="O74" s="30"/>
+      <c r="O74" s="21" t="s">
+        <v>212</v>
+      </c>
       <c r="P74" s="19"/>
       <c r="Q74" s="19"/>
       <c r="R74" s="19"/>
@@ -20574,7 +20588,7 @@
         <v>584</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>574</v>
+        <v>585</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>58</v>
@@ -20585,7 +20599,7 @@
       <c r="I75" s="19"/>
       <c r="J75" s="17"/>
       <c r="K75" s="20">
-        <v>44727.0</v>
+        <v>44856.0</v>
       </c>
       <c r="L75" s="20"/>
       <c r="M75" s="17" t="s">
@@ -20594,9 +20608,7 @@
       <c r="N75" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="O75" s="21" t="s">
-        <v>212</v>
-      </c>
+      <c r="O75" s="30"/>
       <c r="P75" s="19"/>
       <c r="Q75" s="19"/>
       <c r="R75" s="19"/>
@@ -20616,101 +20628,99 @@
       <c r="AF75" s="19"/>
     </row>
     <row r="76">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="K76" s="20"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
+      <c r="A76" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="C76" s="72" t="s">
+        <v>588</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="17"/>
+      <c r="K76" s="20">
+        <v>44727.0</v>
+      </c>
+      <c r="L76" s="20"/>
+      <c r="M76" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N76" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="O76" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="P76" s="19"/>
+      <c r="Q76" s="19"/>
+      <c r="R76" s="19"/>
+      <c r="S76" s="19"/>
+      <c r="T76" s="19"/>
+      <c r="U76" s="19"/>
+      <c r="V76" s="19"/>
+      <c r="W76" s="19"/>
+      <c r="X76" s="19"/>
+      <c r="Y76" s="19"/>
+      <c r="Z76" s="19"/>
+      <c r="AA76" s="19"/>
+      <c r="AB76" s="19"/>
+      <c r="AC76" s="19"/>
+      <c r="AD76" s="19"/>
+      <c r="AE76" s="19"/>
+      <c r="AF76" s="19"/>
     </row>
     <row r="77">
-      <c r="A77" s="8" t="s">
-        <v>585</v>
-      </c>
-      <c r="B77" s="18" t="s">
-        <v>586</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="D77" s="19"/>
-      <c r="E77" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="72"/>
-      <c r="J77" s="17"/>
-      <c r="K77" s="20">
-        <v>43560.0</v>
-      </c>
-      <c r="L77" s="20"/>
-      <c r="M77" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="N77" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="O77" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="P77" s="19"/>
-      <c r="Q77" s="19"/>
-      <c r="R77" s="19"/>
-      <c r="S77" s="19"/>
-      <c r="T77" s="19"/>
-      <c r="U77" s="19"/>
-      <c r="V77" s="19"/>
-      <c r="W77" s="19"/>
-      <c r="X77" s="19"/>
-      <c r="Y77" s="19"/>
-      <c r="Z77" s="19"/>
-      <c r="AA77" s="19"/>
-      <c r="AB77" s="19"/>
-      <c r="AC77" s="19"/>
-      <c r="AD77" s="19"/>
-      <c r="AE77" s="19"/>
-      <c r="AF77" s="19"/>
+      <c r="A77" s="17"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="K77" s="20"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
     </row>
     <row r="78">
-      <c r="A78" s="17" t="s">
-        <v>588</v>
-      </c>
-      <c r="B78" s="22" t="s">
+      <c r="A78" s="8" t="s">
         <v>589</v>
       </c>
+      <c r="B78" s="18" t="s">
+        <v>590</v>
+      </c>
       <c r="C78" s="17" t="s">
-        <v>590</v>
-      </c>
-      <c r="D78" s="17" t="s">
         <v>591</v>
       </c>
+      <c r="D78" s="19"/>
       <c r="E78" s="17" t="s">
         <v>58</v>
       </c>
       <c r="F78" s="19"/>
       <c r="G78" s="19"/>
       <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
-      <c r="J78" s="31" t="s">
-        <v>592</v>
-      </c>
+      <c r="I78" s="72"/>
+      <c r="J78" s="17"/>
       <c r="K78" s="20">
-        <v>44790.0</v>
-      </c>
-      <c r="L78" s="19"/>
-      <c r="M78" s="28" t="s">
+        <v>43560.0</v>
+      </c>
+      <c r="L78" s="20"/>
+      <c r="M78" s="17" t="s">
         <v>20</v>
       </c>
       <c r="N78" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="O78" s="27" t="s">
-        <v>106</v>
+        <v>28</v>
+      </c>
+      <c r="O78" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="P78" s="19"/>
       <c r="Q78" s="19"/>
@@ -20732,16 +20742,16 @@
     </row>
     <row r="79">
       <c r="A79" s="17" t="s">
+        <v>592</v>
+      </c>
+      <c r="B79" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="B79" s="22" t="s">
+      <c r="C79" s="17" t="s">
         <v>594</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="D79" s="17" t="s">
         <v>595</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>591</v>
       </c>
       <c r="E79" s="17" t="s">
         <v>58</v>
@@ -20750,8 +20760,8 @@
       <c r="G79" s="19"/>
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
-      <c r="J79" s="17" t="s">
-        <v>105</v>
+      <c r="J79" s="31" t="s">
+        <v>596</v>
       </c>
       <c r="K79" s="20">
         <v>44790.0</v>
@@ -20786,16 +20796,16 @@
     </row>
     <row r="80">
       <c r="A80" s="17" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="E80" s="17" t="s">
         <v>58</v>
@@ -20840,16 +20850,16 @@
     </row>
     <row r="81">
       <c r="A81" s="17" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="E81" s="17" t="s">
         <v>58</v>
@@ -20858,8 +20868,8 @@
       <c r="G81" s="19"/>
       <c r="H81" s="19"/>
       <c r="I81" s="19"/>
-      <c r="J81" s="31" t="s">
-        <v>602</v>
+      <c r="J81" s="17" t="s">
+        <v>105</v>
       </c>
       <c r="K81" s="20">
         <v>44790.0</v>
@@ -20903,7 +20913,7 @@
         <v>605</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="E82" s="17" t="s">
         <v>58</v>
@@ -20912,8 +20922,8 @@
       <c r="G82" s="19"/>
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
-      <c r="J82" s="17" t="s">
-        <v>105</v>
+      <c r="J82" s="31" t="s">
+        <v>606</v>
       </c>
       <c r="K82" s="20">
         <v>44790.0</v>
@@ -20947,94 +20957,96 @@
       <c r="AF82" s="19"/>
     </row>
     <row r="83">
-      <c r="B83" s="22"/>
-      <c r="C83" s="69"/>
-      <c r="J83" s="49"/>
-      <c r="K83" s="20"/>
-      <c r="M83" s="28"/>
+      <c r="A83" s="17" t="s">
+        <v>607</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>608</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="19"/>
+      <c r="J83" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="K83" s="20">
+        <v>44790.0</v>
+      </c>
+      <c r="L83" s="19"/>
+      <c r="M83" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="N83" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="O83" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="P83" s="19"/>
+      <c r="Q83" s="19"/>
+      <c r="R83" s="19"/>
+      <c r="S83" s="19"/>
+      <c r="T83" s="19"/>
+      <c r="U83" s="19"/>
+      <c r="V83" s="19"/>
+      <c r="W83" s="19"/>
+      <c r="X83" s="19"/>
+      <c r="Y83" s="19"/>
+      <c r="Z83" s="19"/>
+      <c r="AA83" s="19"/>
+      <c r="AB83" s="19"/>
+      <c r="AC83" s="19"/>
+      <c r="AD83" s="19"/>
+      <c r="AE83" s="19"/>
+      <c r="AF83" s="19"/>
     </row>
     <row r="84">
-      <c r="A84" s="99" t="s">
-        <v>606</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>606</v>
-      </c>
-      <c r="C84" s="52" t="s">
-        <v>607</v>
-      </c>
-      <c r="D84" s="13"/>
-      <c r="E84" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="52" t="s">
-        <v>608</v>
-      </c>
-      <c r="J84" s="12"/>
-      <c r="K84" s="14">
-        <v>44461.0</v>
-      </c>
-      <c r="L84" s="33"/>
-      <c r="M84" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N84" s="9" t="s">
-        <v>609</v>
-      </c>
-      <c r="O84" s="53" t="s">
-        <v>347</v>
-      </c>
-      <c r="P84" s="13"/>
-      <c r="Q84" s="13"/>
-      <c r="R84" s="13"/>
-      <c r="S84" s="13"/>
-      <c r="T84" s="13"/>
-      <c r="U84" s="13"/>
-      <c r="V84" s="13"/>
-      <c r="W84" s="13"/>
-      <c r="X84" s="13"/>
-      <c r="Y84" s="13"/>
-      <c r="Z84" s="13"/>
-      <c r="AA84" s="13"/>
-      <c r="AB84" s="13"/>
-      <c r="AC84" s="13"/>
-      <c r="AD84" s="13"/>
-      <c r="AE84" s="13"/>
-      <c r="AF84" s="13"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="69"/>
+      <c r="J84" s="49"/>
+      <c r="K84" s="20"/>
+      <c r="M84" s="28"/>
     </row>
     <row r="85">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="99" t="s">
         <v>610</v>
       </c>
-      <c r="B85" s="51" t="s">
+      <c r="B85" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="C85" s="52" t="s">
         <v>611</v>
       </c>
-      <c r="C85" s="13" t="s">
-        <v>612</v>
-      </c>
-      <c r="D85" s="13" t="s">
-        <v>613</v>
-      </c>
+      <c r="D85" s="13"/>
       <c r="E85" s="52" t="s">
         <v>58</v>
       </c>
       <c r="F85" s="13"/>
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
+      <c r="I85" s="52" t="s">
+        <v>612</v>
+      </c>
+      <c r="J85" s="12"/>
       <c r="K85" s="14">
         <v>44461.0</v>
       </c>
       <c r="L85" s="33"/>
-      <c r="M85" s="13" t="s">
+      <c r="M85" s="12" t="s">
         <v>20</v>
       </c>
       <c r="N85" s="9" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="O85" s="53" t="s">
         <v>347</v>
@@ -21058,177 +21070,175 @@
       <c r="AF85" s="13"/>
     </row>
     <row r="86">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="13" t="s">
         <v>614</v>
       </c>
-      <c r="B86" s="22" t="s">
+      <c r="B86" s="51" t="s">
         <v>615</v>
       </c>
-      <c r="C86" s="17" t="s">
+      <c r="C86" s="13" t="s">
         <v>616</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="E86" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="F86" s="19"/>
-      <c r="G86" s="19"/>
-      <c r="H86" s="19"/>
-      <c r="I86" s="19"/>
-      <c r="J86" s="31" t="s">
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="14">
+        <v>44461.0</v>
+      </c>
+      <c r="L86" s="33"/>
+      <c r="M86" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N86" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="O86" s="53" t="s">
+        <v>347</v>
+      </c>
+      <c r="P86" s="13"/>
+      <c r="Q86" s="13"/>
+      <c r="R86" s="13"/>
+      <c r="S86" s="13"/>
+      <c r="T86" s="13"/>
+      <c r="U86" s="13"/>
+      <c r="V86" s="13"/>
+      <c r="W86" s="13"/>
+      <c r="X86" s="13"/>
+      <c r="Y86" s="13"/>
+      <c r="Z86" s="13"/>
+      <c r="AA86" s="13"/>
+      <c r="AB86" s="13"/>
+      <c r="AC86" s="13"/>
+      <c r="AD86" s="13"/>
+      <c r="AE86" s="13"/>
+      <c r="AF86" s="13"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="17" t="s">
+        <v>618</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>619</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="D87" s="13" t="s">
         <v>617</v>
       </c>
-      <c r="K86" s="20">
+      <c r="E87" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+      <c r="J87" s="31" t="s">
+        <v>621</v>
+      </c>
+      <c r="K87" s="20">
         <v>45429.0</v>
       </c>
-      <c r="L86" s="19"/>
-      <c r="M86" s="17" t="s">
+      <c r="L87" s="19"/>
+      <c r="M87" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N86" s="17" t="s">
+      <c r="N87" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="O86" s="63"/>
-      <c r="P86" s="19"/>
-      <c r="Q86" s="19"/>
-      <c r="R86" s="19"/>
-      <c r="S86" s="19"/>
-      <c r="T86" s="19"/>
-      <c r="U86" s="19"/>
-      <c r="V86" s="19"/>
-      <c r="W86" s="19"/>
-      <c r="X86" s="19"/>
-      <c r="Y86" s="19"/>
-      <c r="Z86" s="19"/>
-      <c r="AA86" s="19"/>
-      <c r="AB86" s="19"/>
-      <c r="AC86" s="19"/>
-      <c r="AD86" s="19"/>
-      <c r="AE86" s="19"/>
-      <c r="AF86" s="19"/>
-    </row>
-    <row r="87">
-      <c r="B87" s="22"/>
-      <c r="J87" s="49"/>
-      <c r="K87" s="20"/>
-      <c r="M87" s="28"/>
+      <c r="O87" s="63"/>
+      <c r="P87" s="19"/>
+      <c r="Q87" s="19"/>
+      <c r="R87" s="19"/>
+      <c r="S87" s="19"/>
+      <c r="T87" s="19"/>
+      <c r="U87" s="19"/>
+      <c r="V87" s="19"/>
+      <c r="W87" s="19"/>
+      <c r="X87" s="19"/>
+      <c r="Y87" s="19"/>
+      <c r="Z87" s="19"/>
+      <c r="AA87" s="19"/>
+      <c r="AB87" s="19"/>
+      <c r="AC87" s="19"/>
+      <c r="AD87" s="19"/>
+      <c r="AE87" s="19"/>
+      <c r="AF87" s="19"/>
     </row>
     <row r="88">
-      <c r="A88" s="8" t="s">
-        <v>618</v>
-      </c>
-      <c r="B88" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>620</v>
-      </c>
-      <c r="D88" s="19"/>
-      <c r="E88" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F88" s="19"/>
-      <c r="G88" s="19"/>
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
-      <c r="J88" s="19"/>
-      <c r="K88" s="20">
-        <v>45396.0</v>
-      </c>
-      <c r="L88" s="20"/>
-      <c r="M88" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="N88" s="74" t="s">
-        <v>621</v>
-      </c>
-      <c r="O88" s="30"/>
-      <c r="P88" s="19"/>
-      <c r="Q88" s="19"/>
-      <c r="R88" s="19"/>
-      <c r="S88" s="19"/>
-      <c r="T88" s="19"/>
-      <c r="U88" s="19"/>
-      <c r="V88" s="19"/>
-      <c r="W88" s="19"/>
-      <c r="X88" s="19"/>
-      <c r="Y88" s="19"/>
-      <c r="Z88" s="19"/>
-      <c r="AA88" s="19"/>
-      <c r="AB88" s="19"/>
-      <c r="AC88" s="19"/>
-      <c r="AD88" s="19"/>
-      <c r="AE88" s="19"/>
-      <c r="AF88" s="19"/>
+      <c r="B88" s="22"/>
+      <c r="J88" s="49"/>
+      <c r="K88" s="20"/>
+      <c r="M88" s="28"/>
     </row>
     <row r="89">
-      <c r="A89" s="100" t="s">
+      <c r="A89" s="8" t="s">
         <v>622</v>
       </c>
-      <c r="B89" s="91" t="s">
+      <c r="B89" s="22" t="s">
         <v>623</v>
       </c>
-      <c r="C89" s="75" t="s">
+      <c r="C89" s="17" t="s">
         <v>624</v>
       </c>
-      <c r="D89" s="100" t="s">
-        <v>625</v>
-      </c>
+      <c r="D89" s="19"/>
       <c r="E89" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F89" s="76"/>
-      <c r="G89" s="91"/>
-      <c r="H89" s="76"/>
-      <c r="I89" s="74" t="s">
-        <v>626</v>
-      </c>
-      <c r="J89" s="91" t="s">
-        <v>627</v>
-      </c>
-      <c r="K89" s="78">
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="19"/>
+      <c r="I89" s="19"/>
+      <c r="J89" s="19"/>
+      <c r="K89" s="20">
         <v>45396.0</v>
       </c>
-      <c r="L89" s="76"/>
+      <c r="L89" s="20"/>
       <c r="M89" s="17" t="s">
         <v>20</v>
       </c>
       <c r="N89" s="74" t="s">
-        <v>621</v>
-      </c>
-      <c r="O89" s="76"/>
-      <c r="P89" s="76"/>
-      <c r="Q89" s="76"/>
-      <c r="R89" s="76"/>
-      <c r="S89" s="76"/>
-      <c r="T89" s="76"/>
-      <c r="U89" s="76"/>
-      <c r="V89" s="76"/>
-      <c r="W89" s="76"/>
-      <c r="X89" s="76"/>
-      <c r="Y89" s="76"/>
-      <c r="Z89" s="76"/>
-      <c r="AA89" s="76"/>
-      <c r="AB89" s="76"/>
-      <c r="AC89" s="76"/>
-      <c r="AD89" s="76"/>
-      <c r="AE89" s="76"/>
-      <c r="AF89" s="76"/>
+        <v>625</v>
+      </c>
+      <c r="O89" s="30"/>
+      <c r="P89" s="19"/>
+      <c r="Q89" s="19"/>
+      <c r="R89" s="19"/>
+      <c r="S89" s="19"/>
+      <c r="T89" s="19"/>
+      <c r="U89" s="19"/>
+      <c r="V89" s="19"/>
+      <c r="W89" s="19"/>
+      <c r="X89" s="19"/>
+      <c r="Y89" s="19"/>
+      <c r="Z89" s="19"/>
+      <c r="AA89" s="19"/>
+      <c r="AB89" s="19"/>
+      <c r="AC89" s="19"/>
+      <c r="AD89" s="19"/>
+      <c r="AE89" s="19"/>
+      <c r="AF89" s="19"/>
     </row>
     <row r="90">
-      <c r="A90" s="83" t="s">
+      <c r="A90" s="100" t="s">
+        <v>626</v>
+      </c>
+      <c r="B90" s="91" t="s">
+        <v>627</v>
+      </c>
+      <c r="C90" s="75" t="s">
         <v>628</v>
       </c>
-      <c r="B90" s="91" t="s">
+      <c r="D90" s="100" t="s">
         <v>629</v>
-      </c>
-      <c r="C90" s="101" t="s">
-        <v>630</v>
-      </c>
-      <c r="D90" s="100" t="s">
-        <v>625</v>
       </c>
       <c r="E90" s="17" t="s">
         <v>58</v>
@@ -21236,7 +21246,9 @@
       <c r="F90" s="76"/>
       <c r="G90" s="91"/>
       <c r="H90" s="76"/>
-      <c r="I90" s="76"/>
+      <c r="I90" s="74" t="s">
+        <v>630</v>
+      </c>
       <c r="J90" s="91" t="s">
         <v>631</v>
       </c>
@@ -21248,7 +21260,7 @@
         <v>20</v>
       </c>
       <c r="N90" s="74" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="O90" s="76"/>
       <c r="P90" s="76"/>
@@ -21270,17 +21282,17 @@
       <c r="AF90" s="76"/>
     </row>
     <row r="91">
-      <c r="A91" s="73" t="s">
+      <c r="A91" s="83" t="s">
         <v>632</v>
       </c>
       <c r="B91" s="91" t="s">
         <v>633</v>
       </c>
-      <c r="C91" s="102" t="s">
+      <c r="C91" s="101" t="s">
         <v>634</v>
       </c>
       <c r="D91" s="100" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="E91" s="17" t="s">
         <v>58</v>
@@ -21288,11 +21300,9 @@
       <c r="F91" s="76"/>
       <c r="G91" s="91"/>
       <c r="H91" s="76"/>
-      <c r="I91" s="74" t="s">
+      <c r="I91" s="76"/>
+      <c r="J91" s="91" t="s">
         <v>635</v>
-      </c>
-      <c r="J91" s="91" t="s">
-        <v>636</v>
       </c>
       <c r="K91" s="78">
         <v>45396.0</v>
@@ -21302,7 +21312,7 @@
         <v>20</v>
       </c>
       <c r="N91" s="74" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="O91" s="76"/>
       <c r="P91" s="76"/>
@@ -21324,118 +21334,122 @@
       <c r="AF91" s="76"/>
     </row>
     <row r="92">
-      <c r="A92" s="103" t="s">
+      <c r="A92" s="73" t="s">
+        <v>636</v>
+      </c>
+      <c r="B92" s="91" t="s">
         <v>637</v>
       </c>
-      <c r="B92" s="104" t="s">
+      <c r="C92" s="102" t="s">
         <v>638</v>
       </c>
-      <c r="C92" s="102" t="s">
-        <v>639</v>
-      </c>
-      <c r="D92" s="105" t="s">
-        <v>640</v>
+      <c r="D92" s="100" t="s">
+        <v>629</v>
       </c>
       <c r="E92" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F92" s="106"/>
-      <c r="G92" s="104"/>
-      <c r="H92" s="106"/>
-      <c r="I92" s="106"/>
-      <c r="J92" s="104" t="s">
-        <v>636</v>
-      </c>
-      <c r="K92" s="107">
+      <c r="F92" s="76"/>
+      <c r="G92" s="91"/>
+      <c r="H92" s="76"/>
+      <c r="I92" s="74" t="s">
+        <v>639</v>
+      </c>
+      <c r="J92" s="91" t="s">
+        <v>640</v>
+      </c>
+      <c r="K92" s="78">
         <v>45396.0</v>
       </c>
-      <c r="L92" s="106"/>
+      <c r="L92" s="76"/>
       <c r="M92" s="17" t="s">
         <v>20</v>
       </c>
       <c r="N92" s="74" t="s">
-        <v>621</v>
-      </c>
-      <c r="O92" s="106"/>
-      <c r="P92" s="106"/>
-      <c r="Q92" s="106"/>
-      <c r="R92" s="106"/>
-      <c r="S92" s="106"/>
-      <c r="T92" s="106"/>
-      <c r="U92" s="106"/>
-      <c r="V92" s="106"/>
-      <c r="W92" s="106"/>
-      <c r="X92" s="106"/>
-      <c r="Y92" s="106"/>
-      <c r="Z92" s="106"/>
-      <c r="AA92" s="106"/>
-      <c r="AB92" s="106"/>
-      <c r="AC92" s="106"/>
-      <c r="AD92" s="106"/>
+        <v>625</v>
+      </c>
+      <c r="O92" s="76"/>
+      <c r="P92" s="76"/>
+      <c r="Q92" s="76"/>
+      <c r="R92" s="76"/>
+      <c r="S92" s="76"/>
+      <c r="T92" s="76"/>
+      <c r="U92" s="76"/>
+      <c r="V92" s="76"/>
+      <c r="W92" s="76"/>
+      <c r="X92" s="76"/>
+      <c r="Y92" s="76"/>
+      <c r="Z92" s="76"/>
+      <c r="AA92" s="76"/>
+      <c r="AB92" s="76"/>
+      <c r="AC92" s="76"/>
+      <c r="AD92" s="76"/>
       <c r="AE92" s="76"/>
       <c r="AF92" s="76"/>
     </row>
-    <row r="94">
-      <c r="A94" s="99" t="s">
+    <row r="93">
+      <c r="A93" s="103" t="s">
         <v>641</v>
       </c>
-      <c r="B94" s="13" t="s">
+      <c r="B93" s="104" t="s">
         <v>642</v>
       </c>
-      <c r="C94" s="108" t="s">
+      <c r="C93" s="102" t="s">
         <v>643</v>
       </c>
-      <c r="D94" s="13" t="s">
+      <c r="D93" s="105" t="s">
         <v>644</v>
       </c>
-      <c r="E94" s="17" t="s">
+      <c r="E93" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="36">
+      <c r="F93" s="106"/>
+      <c r="G93" s="104"/>
+      <c r="H93" s="106"/>
+      <c r="I93" s="106"/>
+      <c r="J93" s="104" t="s">
+        <v>640</v>
+      </c>
+      <c r="K93" s="107">
         <v>45396.0</v>
       </c>
-      <c r="L94" s="13"/>
-      <c r="M94" s="13" t="s">
+      <c r="L93" s="106"/>
+      <c r="M93" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N94" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="O94" s="13"/>
-      <c r="P94" s="13"/>
-      <c r="Q94" s="13"/>
-      <c r="R94" s="13"/>
-      <c r="S94" s="13"/>
-      <c r="T94" s="13"/>
-      <c r="U94" s="13"/>
-      <c r="V94" s="13"/>
-      <c r="W94" s="13"/>
-      <c r="X94" s="13"/>
-      <c r="Y94" s="13"/>
-      <c r="Z94" s="13"/>
-      <c r="AA94" s="13"/>
-      <c r="AB94" s="13"/>
-      <c r="AC94" s="13"/>
-      <c r="AD94" s="13"/>
-      <c r="AE94" s="13"/>
-      <c r="AF94" s="13"/>
+      <c r="N93" s="74" t="s">
+        <v>625</v>
+      </c>
+      <c r="O93" s="106"/>
+      <c r="P93" s="106"/>
+      <c r="Q93" s="106"/>
+      <c r="R93" s="106"/>
+      <c r="S93" s="106"/>
+      <c r="T93" s="106"/>
+      <c r="U93" s="106"/>
+      <c r="V93" s="106"/>
+      <c r="W93" s="106"/>
+      <c r="X93" s="106"/>
+      <c r="Y93" s="106"/>
+      <c r="Z93" s="106"/>
+      <c r="AA93" s="106"/>
+      <c r="AB93" s="106"/>
+      <c r="AC93" s="106"/>
+      <c r="AD93" s="106"/>
+      <c r="AE93" s="76"/>
+      <c r="AF93" s="76"/>
     </row>
     <row r="95">
-      <c r="A95" s="13" t="s">
+      <c r="A95" s="99" t="s">
         <v>645</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>646</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C95" s="108" t="s">
         <v>647</v>
       </c>
-      <c r="D95" s="9" t="s">
+      <c r="D95" s="13" t="s">
         <v>648</v>
       </c>
       <c r="E95" s="17" t="s">
@@ -21444,9 +21458,7 @@
       <c r="F95" s="13"/>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
-      <c r="I95" s="52" t="s">
-        <v>649</v>
-      </c>
+      <c r="I95" s="13"/>
       <c r="J95" s="13"/>
       <c r="K95" s="36">
         <v>45396.0</v>
@@ -21479,16 +21491,16 @@
     </row>
     <row r="96">
       <c r="A96" s="13" t="s">
+        <v>649</v>
+      </c>
+      <c r="B96" s="13" t="s">
         <v>650</v>
       </c>
-      <c r="B96" s="13" t="s">
+      <c r="C96" s="9" t="s">
         <v>651</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="D96" s="9" t="s">
         <v>652</v>
-      </c>
-      <c r="D96" s="13" t="s">
-        <v>653</v>
       </c>
       <c r="E96" s="17" t="s">
         <v>58</v>
@@ -21496,7 +21508,9 @@
       <c r="F96" s="13"/>
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
+      <c r="I96" s="52" t="s">
+        <v>653</v>
+      </c>
       <c r="J96" s="13"/>
       <c r="K96" s="36">
         <v>45396.0</v>
@@ -21537,7 +21551,7 @@
       <c r="C97" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="D97" s="9" t="s">
+      <c r="D97" s="13" t="s">
         <v>657</v>
       </c>
       <c r="E97" s="17" t="s">
@@ -21587,7 +21601,7 @@
       <c r="C98" s="9" t="s">
         <v>660</v>
       </c>
-      <c r="D98" s="13" t="s">
+      <c r="D98" s="9" t="s">
         <v>661</v>
       </c>
       <c r="E98" s="17" t="s">
@@ -21638,7 +21652,7 @@
         <v>664</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="E99" s="17" t="s">
         <v>58</v>
@@ -21646,9 +21660,7 @@
       <c r="F99" s="13"/>
       <c r="G99" s="13"/>
       <c r="H99" s="13"/>
-      <c r="I99" s="52" t="s">
-        <v>665</v>
-      </c>
+      <c r="I99" s="13"/>
       <c r="J99" s="13"/>
       <c r="K99" s="36">
         <v>45396.0</v>
@@ -21690,7 +21702,7 @@
         <v>668</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="E100" s="17" t="s">
         <v>58</v>
@@ -21698,7 +21710,9 @@
       <c r="F100" s="13"/>
       <c r="G100" s="13"/>
       <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
+      <c r="I100" s="52" t="s">
+        <v>669</v>
+      </c>
       <c r="J100" s="13"/>
       <c r="K100" s="36">
         <v>45396.0</v>
@@ -21731,16 +21745,16 @@
     </row>
     <row r="101">
       <c r="A101" s="13" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>671</v>
-      </c>
-      <c r="D101" s="9" t="s">
         <v>672</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>657</v>
       </c>
       <c r="E101" s="17" t="s">
         <v>58</v>
@@ -21789,7 +21803,7 @@
       <c r="C102" s="9" t="s">
         <v>675</v>
       </c>
-      <c r="D102" s="13" t="s">
+      <c r="D102" s="9" t="s">
         <v>676</v>
       </c>
       <c r="E102" s="17" t="s">
@@ -21799,9 +21813,7 @@
       <c r="G102" s="13"/>
       <c r="H102" s="13"/>
       <c r="I102" s="13"/>
-      <c r="J102" s="13" t="s">
-        <v>387</v>
-      </c>
+      <c r="J102" s="13"/>
       <c r="K102" s="36">
         <v>45396.0</v>
       </c>
@@ -21809,8 +21821,8 @@
       <c r="M102" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="N102" s="109" t="s">
-        <v>388</v>
+      <c r="N102" s="52" t="s">
+        <v>53</v>
       </c>
       <c r="O102" s="13"/>
       <c r="P102" s="13"/>
@@ -21832,122 +21844,122 @@
       <c r="AF102" s="13"/>
     </row>
     <row r="103">
-      <c r="A103" s="17" t="s">
+      <c r="A103" s="13" t="s">
         <v>677</v>
       </c>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="13" t="s">
         <v>678</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="9" t="s">
         <v>679</v>
       </c>
       <c r="D103" s="13" t="s">
-        <v>653</v>
+        <v>680</v>
       </c>
       <c r="E103" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F103" s="19"/>
-      <c r="G103" s="19"/>
-      <c r="H103" s="19"/>
-      <c r="I103" s="19"/>
-      <c r="J103" s="19"/>
-      <c r="K103" s="20">
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="K103" s="36">
         <v>45396.0</v>
       </c>
-      <c r="L103" s="19"/>
-      <c r="M103" s="17" t="s">
+      <c r="L103" s="13"/>
+      <c r="M103" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="N103" s="52" t="s">
+      <c r="N103" s="109" t="s">
+        <v>388</v>
+      </c>
+      <c r="O103" s="13"/>
+      <c r="P103" s="13"/>
+      <c r="Q103" s="13"/>
+      <c r="R103" s="13"/>
+      <c r="S103" s="13"/>
+      <c r="T103" s="13"/>
+      <c r="U103" s="13"/>
+      <c r="V103" s="13"/>
+      <c r="W103" s="13"/>
+      <c r="X103" s="13"/>
+      <c r="Y103" s="13"/>
+      <c r="Z103" s="13"/>
+      <c r="AA103" s="13"/>
+      <c r="AB103" s="13"/>
+      <c r="AC103" s="13"/>
+      <c r="AD103" s="13"/>
+      <c r="AE103" s="13"/>
+      <c r="AF103" s="13"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="17" t="s">
+        <v>681</v>
+      </c>
+      <c r="B104" s="17" t="s">
+        <v>682</v>
+      </c>
+      <c r="C104" s="17" t="s">
+        <v>683</v>
+      </c>
+      <c r="D104" s="13" t="s">
+        <v>657</v>
+      </c>
+      <c r="E104" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F104" s="19"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
+      <c r="J104" s="19"/>
+      <c r="K104" s="20">
+        <v>45396.0</v>
+      </c>
+      <c r="L104" s="19"/>
+      <c r="M104" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N104" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="O103" s="19"/>
-      <c r="P103" s="19"/>
-      <c r="Q103" s="19"/>
-      <c r="R103" s="19"/>
-      <c r="S103" s="19"/>
-      <c r="T103" s="19"/>
-      <c r="U103" s="19"/>
-      <c r="V103" s="19"/>
-      <c r="W103" s="19"/>
-      <c r="X103" s="19"/>
-      <c r="Y103" s="19"/>
-      <c r="Z103" s="19"/>
-      <c r="AA103" s="19"/>
-      <c r="AB103" s="19"/>
-      <c r="AC103" s="19"/>
-      <c r="AD103" s="19"/>
-      <c r="AE103" s="19"/>
-      <c r="AF103" s="19"/>
-    </row>
-    <row r="104">
-      <c r="B104" s="22"/>
-      <c r="K104" s="20"/>
+      <c r="O104" s="19"/>
+      <c r="P104" s="19"/>
+      <c r="Q104" s="19"/>
+      <c r="R104" s="19"/>
+      <c r="S104" s="19"/>
+      <c r="T104" s="19"/>
+      <c r="U104" s="19"/>
+      <c r="V104" s="19"/>
+      <c r="W104" s="19"/>
+      <c r="X104" s="19"/>
+      <c r="Y104" s="19"/>
+      <c r="Z104" s="19"/>
+      <c r="AA104" s="19"/>
+      <c r="AB104" s="19"/>
+      <c r="AC104" s="19"/>
+      <c r="AD104" s="19"/>
+      <c r="AE104" s="19"/>
+      <c r="AF104" s="19"/>
     </row>
     <row r="105">
-      <c r="A105" s="99" t="s">
-        <v>680</v>
-      </c>
-      <c r="B105" s="13" t="s">
-        <v>681</v>
-      </c>
-      <c r="C105" s="70" t="s">
-        <v>682</v>
-      </c>
-      <c r="D105" s="13"/>
-      <c r="E105" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F105" s="13"/>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="13"/>
-      <c r="J105" s="13" t="s">
-        <v>683</v>
-      </c>
-      <c r="K105" s="36">
-        <v>45396.0</v>
-      </c>
-      <c r="L105" s="13"/>
-      <c r="M105" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="N105" s="109" t="s">
-        <v>388</v>
-      </c>
-      <c r="O105" s="13"/>
-      <c r="P105" s="13"/>
-      <c r="Q105" s="13"/>
-      <c r="R105" s="13"/>
-      <c r="S105" s="13"/>
-      <c r="T105" s="13"/>
-      <c r="U105" s="13"/>
-      <c r="V105" s="13"/>
-      <c r="W105" s="13"/>
-      <c r="X105" s="13"/>
-      <c r="Y105" s="13"/>
-      <c r="Z105" s="13"/>
-      <c r="AA105" s="13"/>
-      <c r="AB105" s="13"/>
-      <c r="AC105" s="13"/>
-      <c r="AD105" s="13"/>
-      <c r="AE105" s="13"/>
-      <c r="AF105" s="13"/>
+      <c r="B105" s="22"/>
+      <c r="K105" s="20"/>
     </row>
     <row r="106">
-      <c r="A106" s="13" t="s">
+      <c r="A106" s="99" t="s">
         <v>684</v>
       </c>
       <c r="B106" s="13" t="s">
         <v>685</v>
       </c>
-      <c r="C106" s="108" t="s">
+      <c r="C106" s="70" t="s">
         <v>686</v>
       </c>
-      <c r="D106" s="13" t="s">
-        <v>687</v>
-      </c>
+      <c r="D106" s="13"/>
       <c r="E106" s="17" t="s">
         <v>58</v>
       </c>
@@ -21956,7 +21968,7 @@
       <c r="H106" s="13"/>
       <c r="I106" s="13"/>
       <c r="J106" s="13" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="K106" s="36">
         <v>45396.0</v>
@@ -21994,11 +22006,11 @@
       <c r="B107" s="13" t="s">
         <v>689</v>
       </c>
-      <c r="C107" s="70" t="s">
+      <c r="C107" s="108" t="s">
         <v>690</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="E107" s="17" t="s">
         <v>58</v>
@@ -22008,7 +22020,7 @@
       <c r="H107" s="13"/>
       <c r="I107" s="13"/>
       <c r="J107" s="13" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="K107" s="36">
         <v>45396.0</v>
@@ -22041,16 +22053,16 @@
     </row>
     <row r="108">
       <c r="A108" s="13" t="s">
+        <v>692</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>693</v>
+      </c>
+      <c r="C108" s="70" t="s">
+        <v>694</v>
+      </c>
+      <c r="D108" s="13" t="s">
         <v>691</v>
-      </c>
-      <c r="B108" s="13" t="s">
-        <v>692</v>
-      </c>
-      <c r="C108" s="70" t="s">
-        <v>693</v>
-      </c>
-      <c r="D108" s="13" t="s">
-        <v>687</v>
       </c>
       <c r="E108" s="17" t="s">
         <v>58</v>
@@ -22060,7 +22072,7 @@
       <c r="H108" s="13"/>
       <c r="I108" s="13"/>
       <c r="J108" s="13" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="K108" s="36">
         <v>45396.0</v>
@@ -22091,62 +22103,70 @@
       <c r="AE108" s="13"/>
       <c r="AF108" s="13"/>
     </row>
-    <row r="110">
-      <c r="A110" s="100"/>
-      <c r="B110" s="91"/>
-      <c r="C110" s="101"/>
-      <c r="D110" s="83"/>
-      <c r="F110" s="76"/>
-      <c r="G110" s="91"/>
-      <c r="H110" s="76"/>
-      <c r="I110" s="76"/>
-      <c r="J110" s="91"/>
-      <c r="K110" s="76"/>
-      <c r="L110" s="76"/>
-      <c r="N110" s="76"/>
-      <c r="O110" s="76"/>
-      <c r="P110" s="76"/>
-      <c r="Q110" s="76"/>
-      <c r="R110" s="76"/>
-      <c r="S110" s="76"/>
-      <c r="T110" s="76"/>
-      <c r="U110" s="76"/>
-      <c r="V110" s="76"/>
-      <c r="W110" s="76"/>
-      <c r="X110" s="76"/>
-      <c r="Y110" s="76"/>
-      <c r="Z110" s="76"/>
-      <c r="AA110" s="76"/>
-      <c r="AB110" s="76"/>
-      <c r="AC110" s="76"/>
-      <c r="AD110" s="76"/>
-      <c r="AE110" s="76"/>
-      <c r="AF110" s="76"/>
+    <row r="109">
+      <c r="A109" s="13" t="s">
+        <v>695</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>696</v>
+      </c>
+      <c r="C109" s="70" t="s">
+        <v>697</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>691</v>
+      </c>
+      <c r="E109" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F109" s="13"/>
+      <c r="G109" s="13"/>
+      <c r="H109" s="13"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="13" t="s">
+        <v>687</v>
+      </c>
+      <c r="K109" s="36">
+        <v>45396.0</v>
+      </c>
+      <c r="L109" s="13"/>
+      <c r="M109" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N109" s="109" t="s">
+        <v>388</v>
+      </c>
+      <c r="O109" s="13"/>
+      <c r="P109" s="13"/>
+      <c r="Q109" s="13"/>
+      <c r="R109" s="13"/>
+      <c r="S109" s="13"/>
+      <c r="T109" s="13"/>
+      <c r="U109" s="13"/>
+      <c r="V109" s="13"/>
+      <c r="W109" s="13"/>
+      <c r="X109" s="13"/>
+      <c r="Y109" s="13"/>
+      <c r="Z109" s="13"/>
+      <c r="AA109" s="13"/>
+      <c r="AB109" s="13"/>
+      <c r="AC109" s="13"/>
+      <c r="AD109" s="13"/>
+      <c r="AE109" s="13"/>
+      <c r="AF109" s="13"/>
     </row>
     <row r="111">
-      <c r="A111" s="76" t="s">
-        <v>694</v>
-      </c>
-      <c r="B111" s="76" t="s">
-        <v>695</v>
-      </c>
-      <c r="C111" s="96" t="s">
-        <v>696</v>
-      </c>
-      <c r="D111" s="76"/>
-      <c r="E111" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="A111" s="100"/>
+      <c r="B111" s="91"/>
+      <c r="C111" s="101"/>
+      <c r="D111" s="83"/>
       <c r="F111" s="76"/>
-      <c r="G111" s="76"/>
+      <c r="G111" s="91"/>
       <c r="H111" s="76"/>
       <c r="I111" s="76"/>
-      <c r="J111" s="76"/>
+      <c r="J111" s="91"/>
       <c r="K111" s="76"/>
       <c r="L111" s="76"/>
-      <c r="M111" s="17" t="s">
-        <v>697</v>
-      </c>
       <c r="N111" s="76"/>
       <c r="O111" s="76"/>
       <c r="P111" s="76"/>
@@ -22164,39 +22184,37 @@
       <c r="AB111" s="76"/>
       <c r="AC111" s="76"/>
       <c r="AD111" s="76"/>
+      <c r="AE111" s="76"/>
+      <c r="AF111" s="76"/>
     </row>
     <row r="112">
-      <c r="A112" s="80" t="s">
+      <c r="A112" s="76" t="s">
         <v>698</v>
       </c>
-      <c r="B112" s="86"/>
-      <c r="C112" s="82" t="s">
+      <c r="B112" s="76" t="s">
         <v>699</v>
       </c>
-      <c r="D112" s="110" t="s">
-        <v>51</v>
-      </c>
-      <c r="E112" s="84" t="s">
+      <c r="C112" s="96" t="s">
+        <v>700</v>
+      </c>
+      <c r="D112" s="76"/>
+      <c r="E112" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F112" s="85"/>
-      <c r="G112" s="85"/>
-      <c r="H112" s="85"/>
-      <c r="I112" s="86"/>
-      <c r="J112" s="86"/>
-      <c r="K112" s="78">
-        <v>45396.0</v>
-      </c>
-      <c r="L112" s="87"/>
-      <c r="M112" s="74" t="s">
-        <v>697</v>
-      </c>
-      <c r="N112" s="82" t="s">
-        <v>211</v>
-      </c>
-      <c r="O112" s="86"/>
-      <c r="P112" s="85"/>
-      <c r="Q112" s="85"/>
+      <c r="F112" s="76"/>
+      <c r="G112" s="76"/>
+      <c r="H112" s="76"/>
+      <c r="I112" s="76"/>
+      <c r="J112" s="76"/>
+      <c r="K112" s="76"/>
+      <c r="L112" s="76"/>
+      <c r="M112" s="17" t="s">
+        <v>701</v>
+      </c>
+      <c r="N112" s="76"/>
+      <c r="O112" s="76"/>
+      <c r="P112" s="76"/>
+      <c r="Q112" s="76"/>
       <c r="R112" s="76"/>
       <c r="S112" s="76"/>
       <c r="T112" s="76"/>
@@ -22210,74 +22228,70 @@
       <c r="AB112" s="76"/>
       <c r="AC112" s="76"/>
       <c r="AD112" s="76"/>
-      <c r="AE112" s="76"/>
-      <c r="AF112" s="76"/>
     </row>
     <row r="113">
-      <c r="B113" s="22"/>
-      <c r="N113" s="111"/>
+      <c r="A113" s="80" t="s">
+        <v>702</v>
+      </c>
+      <c r="B113" s="86"/>
+      <c r="C113" s="82" t="s">
+        <v>703</v>
+      </c>
+      <c r="D113" s="110" t="s">
+        <v>51</v>
+      </c>
+      <c r="E113" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="F113" s="85"/>
+      <c r="G113" s="85"/>
+      <c r="H113" s="85"/>
+      <c r="I113" s="86"/>
+      <c r="J113" s="86"/>
+      <c r="K113" s="78">
+        <v>45396.0</v>
+      </c>
+      <c r="L113" s="87"/>
+      <c r="M113" s="74" t="s">
+        <v>701</v>
+      </c>
+      <c r="N113" s="82" t="s">
+        <v>211</v>
+      </c>
+      <c r="O113" s="86"/>
+      <c r="P113" s="85"/>
+      <c r="Q113" s="85"/>
+      <c r="R113" s="76"/>
+      <c r="S113" s="76"/>
+      <c r="T113" s="76"/>
+      <c r="U113" s="76"/>
+      <c r="V113" s="76"/>
+      <c r="W113" s="76"/>
+      <c r="X113" s="76"/>
+      <c r="Y113" s="76"/>
+      <c r="Z113" s="76"/>
+      <c r="AA113" s="76"/>
+      <c r="AB113" s="76"/>
+      <c r="AC113" s="76"/>
+      <c r="AD113" s="76"/>
+      <c r="AE113" s="76"/>
+      <c r="AF113" s="76"/>
     </row>
     <row r="114">
-      <c r="A114" s="17" t="s">
-        <v>700</v>
-      </c>
-      <c r="B114" s="17" t="s">
-        <v>701</v>
-      </c>
-      <c r="C114" s="17" t="s">
-        <v>702</v>
-      </c>
-      <c r="D114" s="19"/>
-      <c r="E114" s="84" t="s">
-        <v>58</v>
-      </c>
-      <c r="F114" s="19"/>
-      <c r="G114" s="19"/>
-      <c r="H114" s="19"/>
-      <c r="I114" s="19"/>
-      <c r="J114" s="19"/>
-      <c r="K114" s="20">
-        <v>45429.0</v>
-      </c>
-      <c r="L114" s="19"/>
-      <c r="M114" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="N114" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="O114" s="19"/>
-      <c r="P114" s="19"/>
-      <c r="Q114" s="19"/>
-      <c r="R114" s="19"/>
-      <c r="S114" s="19"/>
-      <c r="T114" s="19"/>
-      <c r="U114" s="19"/>
-      <c r="V114" s="19"/>
-      <c r="W114" s="19"/>
-      <c r="X114" s="19"/>
-      <c r="Y114" s="19"/>
-      <c r="Z114" s="19"/>
-      <c r="AA114" s="19"/>
-      <c r="AB114" s="19"/>
-      <c r="AC114" s="19"/>
-      <c r="AD114" s="19"/>
-      <c r="AE114" s="19"/>
-      <c r="AF114" s="19"/>
+      <c r="B114" s="22"/>
+      <c r="N114" s="111"/>
     </row>
     <row r="115">
       <c r="A115" s="17" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>705</v>
-      </c>
-      <c r="D115" s="17" t="s">
         <v>706</v>
       </c>
+      <c r="D115" s="19"/>
       <c r="E115" s="84" t="s">
         <v>58</v>
       </c>
@@ -22326,7 +22340,7 @@
         <v>709</v>
       </c>
       <c r="D116" s="17" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
       <c r="E116" s="84" t="s">
         <v>58</v>
@@ -22365,50 +22379,62 @@
       <c r="AE116" s="19"/>
       <c r="AF116" s="19"/>
     </row>
-    <row r="119">
-      <c r="A119" s="112" t="s">
+    <row r="117">
+      <c r="A117" s="17" t="s">
+        <v>711</v>
+      </c>
+      <c r="B117" s="17" t="s">
+        <v>712</v>
+      </c>
+      <c r="C117" s="17" t="s">
+        <v>713</v>
+      </c>
+      <c r="D117" s="17" t="s">
         <v>710</v>
       </c>
-      <c r="B119" s="76"/>
-      <c r="C119" s="76"/>
-      <c r="D119" s="76"/>
-      <c r="E119" s="76"/>
-      <c r="F119" s="76"/>
-      <c r="G119" s="76"/>
-      <c r="H119" s="76"/>
-      <c r="I119" s="76"/>
-      <c r="J119" s="76"/>
-      <c r="K119" s="79"/>
-      <c r="L119" s="79"/>
-      <c r="M119" s="76"/>
-      <c r="N119" s="76"/>
-      <c r="O119" s="76"/>
-      <c r="P119" s="76"/>
-      <c r="Q119" s="76"/>
-      <c r="R119" s="76"/>
-      <c r="S119" s="76"/>
-      <c r="T119" s="76"/>
-      <c r="U119" s="76"/>
-      <c r="V119" s="76"/>
-      <c r="W119" s="76"/>
-      <c r="X119" s="76"/>
-      <c r="Y119" s="76"/>
-      <c r="Z119" s="76"/>
-      <c r="AA119" s="76"/>
-      <c r="AB119" s="76"/>
-      <c r="AC119" s="76"/>
-      <c r="AD119" s="76"/>
+      <c r="E117" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="F117" s="19"/>
+      <c r="G117" s="19"/>
+      <c r="H117" s="19"/>
+      <c r="I117" s="19"/>
+      <c r="J117" s="19"/>
+      <c r="K117" s="20">
+        <v>45429.0</v>
+      </c>
+      <c r="L117" s="19"/>
+      <c r="M117" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N117" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="O117" s="19"/>
+      <c r="P117" s="19"/>
+      <c r="Q117" s="19"/>
+      <c r="R117" s="19"/>
+      <c r="S117" s="19"/>
+      <c r="T117" s="19"/>
+      <c r="U117" s="19"/>
+      <c r="V117" s="19"/>
+      <c r="W117" s="19"/>
+      <c r="X117" s="19"/>
+      <c r="Y117" s="19"/>
+      <c r="Z117" s="19"/>
+      <c r="AA117" s="19"/>
+      <c r="AB117" s="19"/>
+      <c r="AC117" s="19"/>
+      <c r="AD117" s="19"/>
+      <c r="AE117" s="19"/>
+      <c r="AF117" s="19"/>
     </row>
     <row r="120">
-      <c r="A120" s="76" t="s">
-        <v>407</v>
-      </c>
-      <c r="B120" s="76" t="s">
-        <v>711</v>
-      </c>
-      <c r="C120" s="76" t="s">
-        <v>712</v>
-      </c>
+      <c r="A120" s="112" t="s">
+        <v>714</v>
+      </c>
+      <c r="B120" s="76"/>
+      <c r="C120" s="76"/>
       <c r="D120" s="76"/>
       <c r="E120" s="76"/>
       <c r="F120" s="76"/>
@@ -22439,17 +22465,15 @@
     </row>
     <row r="121">
       <c r="A121" s="76" t="s">
-        <v>713</v>
+        <v>407</v>
       </c>
       <c r="B121" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C121" s="76" t="s">
-        <v>714</v>
-      </c>
-      <c r="D121" s="76" t="s">
-        <v>711</v>
-      </c>
+        <v>716</v>
+      </c>
+      <c r="D121" s="76"/>
       <c r="E121" s="76"/>
       <c r="F121" s="76"/>
       <c r="G121" s="76"/>
@@ -22479,15 +22503,17 @@
     </row>
     <row r="122">
       <c r="A122" s="76" t="s">
+        <v>717</v>
+      </c>
+      <c r="B122" s="76" t="s">
         <v>715</v>
       </c>
-      <c r="B122" s="76" t="s">
-        <v>711</v>
-      </c>
       <c r="C122" s="76" t="s">
-        <v>716</v>
-      </c>
-      <c r="D122" s="76"/>
+        <v>718</v>
+      </c>
+      <c r="D122" s="76" t="s">
+        <v>715</v>
+      </c>
       <c r="E122" s="76"/>
       <c r="F122" s="76"/>
       <c r="G122" s="76"/>
@@ -22517,13 +22543,13 @@
     </row>
     <row r="123">
       <c r="A123" s="76" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B123" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C123" s="76" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="D123" s="76"/>
       <c r="E123" s="76"/>
@@ -22555,12 +22581,14 @@
     </row>
     <row r="124">
       <c r="A124" s="76" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B124" s="76" t="s">
-        <v>711</v>
-      </c>
-      <c r="C124" s="76"/>
+        <v>715</v>
+      </c>
+      <c r="C124" s="76" t="s">
+        <v>722</v>
+      </c>
       <c r="D124" s="76"/>
       <c r="E124" s="76"/>
       <c r="F124" s="76"/>
@@ -22591,10 +22619,10 @@
     </row>
     <row r="125">
       <c r="A125" s="76" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="B125" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C125" s="76"/>
       <c r="D125" s="76"/>
@@ -22627,10 +22655,10 @@
     </row>
     <row r="126">
       <c r="A126" s="76" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B126" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C126" s="76"/>
       <c r="D126" s="76"/>
@@ -22663,10 +22691,10 @@
     </row>
     <row r="127">
       <c r="A127" s="76" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="B127" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C127" s="76"/>
       <c r="D127" s="76"/>
@@ -22699,10 +22727,10 @@
     </row>
     <row r="128">
       <c r="A128" s="76" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="B128" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C128" s="76"/>
       <c r="D128" s="76"/>
@@ -22735,10 +22763,10 @@
     </row>
     <row r="129">
       <c r="A129" s="76" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="B129" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C129" s="76"/>
       <c r="D129" s="76"/>
@@ -22771,10 +22799,10 @@
     </row>
     <row r="130">
       <c r="A130" s="76" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B130" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C130" s="76"/>
       <c r="D130" s="76"/>
@@ -22807,10 +22835,10 @@
     </row>
     <row r="131">
       <c r="A131" s="76" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="B131" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C131" s="76"/>
       <c r="D131" s="76"/>
@@ -22843,10 +22871,10 @@
     </row>
     <row r="132">
       <c r="A132" s="76" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="B132" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C132" s="76"/>
       <c r="D132" s="76"/>
@@ -22879,10 +22907,10 @@
     </row>
     <row r="133">
       <c r="A133" s="76" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B133" s="76" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C133" s="76"/>
       <c r="D133" s="76"/>
@@ -22915,10 +22943,10 @@
     </row>
     <row r="134">
       <c r="A134" s="76" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="B134" s="76" t="s">
-        <v>730</v>
+        <v>715</v>
       </c>
       <c r="C134" s="76"/>
       <c r="D134" s="76"/>
@@ -22951,10 +22979,10 @@
     </row>
     <row r="135">
       <c r="A135" s="76" t="s">
-        <v>36</v>
+        <v>733</v>
       </c>
       <c r="B135" s="76" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="C135" s="76"/>
       <c r="D135" s="76"/>
@@ -22987,9 +23015,11 @@
     </row>
     <row r="136">
       <c r="A136" s="76" t="s">
-        <v>732</v>
-      </c>
-      <c r="B136" s="76"/>
+        <v>36</v>
+      </c>
+      <c r="B136" s="76" t="s">
+        <v>735</v>
+      </c>
       <c r="C136" s="76"/>
       <c r="D136" s="76"/>
       <c r="E136" s="76"/>
@@ -23021,7 +23051,7 @@
     </row>
     <row r="137">
       <c r="A137" s="76" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="B137" s="76"/>
       <c r="C137" s="76"/>
@@ -23055,7 +23085,7 @@
     </row>
     <row r="138">
       <c r="A138" s="76" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="B138" s="76"/>
       <c r="C138" s="76"/>
@@ -23089,7 +23119,7 @@
     </row>
     <row r="139">
       <c r="A139" s="76" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="B139" s="76"/>
       <c r="C139" s="76"/>
@@ -23123,7 +23153,7 @@
     </row>
     <row r="140">
       <c r="A140" s="76" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="B140" s="76"/>
       <c r="C140" s="76"/>
@@ -23156,7 +23186,9 @@
       <c r="AD140" s="76"/>
     </row>
     <row r="141">
-      <c r="A141" s="76"/>
+      <c r="A141" s="76" t="s">
+        <v>740</v>
+      </c>
       <c r="B141" s="76"/>
       <c r="C141" s="76"/>
       <c r="D141" s="76"/>
@@ -23188,13 +23220,9 @@
       <c r="AD141" s="76"/>
     </row>
     <row r="142">
-      <c r="A142" s="76" t="s">
-        <v>737</v>
-      </c>
+      <c r="A142" s="76"/>
       <c r="B142" s="76"/>
-      <c r="C142" s="76" t="s">
-        <v>738</v>
-      </c>
+      <c r="C142" s="76"/>
       <c r="D142" s="76"/>
       <c r="E142" s="76"/>
       <c r="F142" s="76"/>
@@ -23224,7 +23252,40 @@
       <c r="AD142" s="76"/>
     </row>
     <row r="143">
-      <c r="B143" s="23"/>
+      <c r="A143" s="76" t="s">
+        <v>741</v>
+      </c>
+      <c r="B143" s="76"/>
+      <c r="C143" s="76" t="s">
+        <v>742</v>
+      </c>
+      <c r="D143" s="76"/>
+      <c r="E143" s="76"/>
+      <c r="F143" s="76"/>
+      <c r="G143" s="76"/>
+      <c r="H143" s="76"/>
+      <c r="I143" s="76"/>
+      <c r="J143" s="76"/>
+      <c r="K143" s="79"/>
+      <c r="L143" s="79"/>
+      <c r="M143" s="76"/>
+      <c r="N143" s="76"/>
+      <c r="O143" s="76"/>
+      <c r="P143" s="76"/>
+      <c r="Q143" s="76"/>
+      <c r="R143" s="76"/>
+      <c r="S143" s="76"/>
+      <c r="T143" s="76"/>
+      <c r="U143" s="76"/>
+      <c r="V143" s="76"/>
+      <c r="W143" s="76"/>
+      <c r="X143" s="76"/>
+      <c r="Y143" s="76"/>
+      <c r="Z143" s="76"/>
+      <c r="AA143" s="76"/>
+      <c r="AB143" s="76"/>
+      <c r="AC143" s="76"/>
+      <c r="AD143" s="76"/>
     </row>
     <row r="144">
       <c r="B144" s="23"/>
@@ -25731,18 +25792,21 @@
     <row r="978">
       <c r="B978" s="23"/>
     </row>
+    <row r="979">
+      <c r="B979" s="23"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AF208">
+  <conditionalFormatting sqref="A2:AF209">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Q211">
+  <conditionalFormatting sqref="A1:Q212">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>$M1="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Q211">
+  <conditionalFormatting sqref="A1:Q212">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>$M1="changed"</formula>
     </cfRule>
@@ -25797,25 +25861,26 @@
     <hyperlink r:id="rId47" ref="O63"/>
     <hyperlink r:id="rId48" ref="O64"/>
     <hyperlink r:id="rId49" ref="O65"/>
-    <hyperlink r:id="rId50" ref="I66"/>
-    <hyperlink r:id="rId51" ref="O66"/>
-    <hyperlink r:id="rId52" ref="O71"/>
+    <hyperlink r:id="rId50" ref="O66"/>
+    <hyperlink r:id="rId51" ref="I67"/>
+    <hyperlink r:id="rId52" ref="O67"/>
     <hyperlink r:id="rId53" ref="O72"/>
     <hyperlink r:id="rId54" ref="O73"/>
-    <hyperlink r:id="rId55" ref="O75"/>
-    <hyperlink r:id="rId56" ref="O77"/>
-    <hyperlink r:id="rId57" ref="J78"/>
-    <hyperlink r:id="rId58" ref="O78"/>
+    <hyperlink r:id="rId55" ref="O74"/>
+    <hyperlink r:id="rId56" ref="O76"/>
+    <hyperlink r:id="rId57" ref="O78"/>
+    <hyperlink r:id="rId58" ref="J79"/>
     <hyperlink r:id="rId59" ref="O79"/>
     <hyperlink r:id="rId60" ref="O80"/>
-    <hyperlink r:id="rId61" ref="J81"/>
-    <hyperlink r:id="rId62" ref="O81"/>
+    <hyperlink r:id="rId61" ref="O81"/>
+    <hyperlink r:id="rId62" ref="J82"/>
     <hyperlink r:id="rId63" ref="O82"/>
-    <hyperlink r:id="rId64" ref="O84"/>
+    <hyperlink r:id="rId64" ref="O83"/>
     <hyperlink r:id="rId65" ref="O85"/>
-    <hyperlink r:id="rId66" ref="J86"/>
+    <hyperlink r:id="rId66" ref="O86"/>
+    <hyperlink r:id="rId67" ref="J87"/>
   </hyperlinks>
-  <drawing r:id="rId67"/>
+  <drawing r:id="rId68"/>
 </worksheet>
 </file>
 
@@ -25887,13 +25952,13 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="17" t="s">
@@ -25936,16 +26001,16 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>81</v>
@@ -25999,16 +26064,16 @@
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>81</v>
@@ -26017,7 +26082,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="17" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="20">
@@ -26028,7 +26093,7 @@
         <v>20</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="O5" s="68" t="s">
         <v>63</v>
@@ -26052,16 +26117,16 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>81</v>
@@ -26079,7 +26144,7 @@
         <v>20</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="O6" s="68" t="s">
         <v>63</v>
@@ -26103,16 +26168,16 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>81</v>
@@ -26130,7 +26195,7 @@
         <v>20</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="O7" s="68" t="s">
         <v>63</v>
@@ -26154,16 +26219,16 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
+        <v>762</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>763</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>764</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>758</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>759</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>760</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>754</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>81</v>
@@ -26181,7 +26246,7 @@
         <v>20</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="O8" s="68" t="s">
         <v>63</v>
@@ -26205,16 +26270,16 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>81</v>
@@ -26289,16 +26354,16 @@
     </row>
     <row r="11">
       <c r="A11" s="113" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="B11" s="83" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="C11" s="75" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
       <c r="D11" s="83" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>81</v>
@@ -26308,7 +26373,7 @@
       <c r="H11" s="76"/>
       <c r="I11" s="76"/>
       <c r="J11" s="91" t="s">
-        <v>767</v>
+        <v>771</v>
       </c>
       <c r="K11" s="20">
         <v>44601.0</v>
@@ -26338,16 +26403,16 @@
     </row>
     <row r="12">
       <c r="A12" s="114" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
       <c r="D12" s="83" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>81</v>
@@ -26385,16 +26450,16 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>81</v>
@@ -26439,30 +26504,30 @@
     </row>
     <row r="15">
       <c r="A15" s="113" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="B15" s="83" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>775</v>
+        <v>779</v>
       </c>
       <c r="D15" s="91" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>81</v>
       </c>
       <c r="F15" s="76"/>
       <c r="G15" s="91" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
       <c r="H15" s="91" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c r="I15" s="76"/>
       <c r="J15" s="91" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="K15" s="20">
         <v>44601.0</v>
@@ -29200,13 +29265,13 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>104</v>
@@ -29219,7 +29284,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="17" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c r="K2" s="20">
         <v>44727.0</v>
@@ -29253,13 +29318,13 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="17" t="s">
@@ -29270,7 +29335,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="17" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="K3" s="67">
         <v>45396.0</v>
@@ -29302,13 +29367,13 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="17" t="s">
@@ -29319,7 +29384,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="90"/>
       <c r="J4" s="17" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="K4" s="67">
         <v>45396.0</v>
@@ -29351,13 +29416,13 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="17" t="s">
@@ -29368,7 +29433,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="17" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="K5" s="67">
         <v>45396.0</v>
@@ -29400,13 +29465,13 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="17" t="s">
@@ -29417,7 +29482,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="17" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="K6" s="67">
         <v>45396.0</v>
@@ -29449,13 +29514,13 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="17" t="s">
@@ -29466,7 +29531,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="17" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="K7" s="67">
         <v>45396.0</v>
@@ -29498,13 +29563,13 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="17" t="s">
@@ -29515,7 +29580,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="17" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="K8" s="67">
         <v>45396.0</v>
@@ -29547,13 +29612,13 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="17" t="s">
@@ -29564,7 +29629,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="17" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="K9" s="67">
         <v>45396.0</v>
@@ -29596,13 +29661,13 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>814</v>
+        <v>818</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="17" t="s">
@@ -29613,7 +29678,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="17" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c r="K10" s="67">
         <v>45396.0</v>
@@ -29645,13 +29710,13 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>817</v>
+        <v>821</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="17" t="s">
@@ -29662,7 +29727,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="17" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
       <c r="K11" s="67">
         <v>45396.0</v>
@@ -29694,13 +29759,13 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>820</v>
+        <v>824</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>822</v>
+        <v>826</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="17" t="s">
@@ -29711,7 +29776,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="17" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
       <c r="K12" s="67">
         <v>45396.0</v>
@@ -33313,13 +33378,13 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="17" t="s">
@@ -33329,7 +33394,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="17" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="20">
@@ -33337,7 +33402,7 @@
       </c>
       <c r="L2" s="19"/>
       <c r="M2" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>53</v>
@@ -33359,13 +33424,13 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>827</v>
+        <v>831</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="17" t="s">
@@ -33381,7 +33446,7 @@
       </c>
       <c r="L3" s="19"/>
       <c r="M3" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N3" s="17" t="s">
         <v>53</v>
@@ -33403,13 +33468,13 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>830</v>
+        <v>834</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="17" t="s">
@@ -33419,7 +33484,7 @@
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
       <c r="I4" s="17" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="20">
@@ -33427,7 +33492,7 @@
       </c>
       <c r="L4" s="19"/>
       <c r="M4" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N4" s="17" t="s">
         <v>53</v>
@@ -33438,13 +33503,13 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>836</v>
+        <v>840</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="17" t="s">
@@ -33454,7 +33519,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="90" t="s">
-        <v>837</v>
+        <v>841</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="20">
@@ -33462,7 +33527,7 @@
       </c>
       <c r="L5" s="19"/>
       <c r="M5" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N5" s="17" t="s">
         <v>53</v>
@@ -33473,13 +33538,13 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="17" t="s">
@@ -33489,7 +33554,7 @@
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="17" t="s">
-        <v>841</v>
+        <v>845</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="20">
@@ -33497,7 +33562,7 @@
       </c>
       <c r="L6" s="19"/>
       <c r="M6" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N6" s="17" t="s">
         <v>53</v>
@@ -33508,13 +33573,13 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="17" t="s">
@@ -33524,7 +33589,7 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="17" t="s">
-        <v>845</v>
+        <v>849</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="20">
@@ -33532,7 +33597,7 @@
       </c>
       <c r="L7" s="19"/>
       <c r="M7" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>53</v>
@@ -33543,13 +33608,13 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="17" t="s">
@@ -33559,7 +33624,7 @@
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="17" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="J8" s="19"/>
       <c r="K8" s="20">
@@ -33567,7 +33632,7 @@
       </c>
       <c r="L8" s="19"/>
       <c r="M8" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N8" s="17" t="s">
         <v>53</v>
@@ -33578,13 +33643,13 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="17" t="s">
@@ -33600,7 +33665,7 @@
       </c>
       <c r="L9" s="19"/>
       <c r="M9" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N9" s="17" t="s">
         <v>53</v>
@@ -33611,13 +33676,13 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="17" t="s">
@@ -33633,7 +33698,7 @@
       </c>
       <c r="L10" s="19"/>
       <c r="M10" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N10" s="17" t="s">
         <v>53</v>
@@ -33644,13 +33709,13 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="17" t="s">
@@ -33666,7 +33731,7 @@
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N11" s="17" t="s">
         <v>53</v>
@@ -33677,13 +33742,13 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="17" t="s">
@@ -33699,7 +33764,7 @@
       </c>
       <c r="L12" s="19"/>
       <c r="M12" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N12" s="17" t="s">
         <v>53</v>
@@ -33710,13 +33775,13 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="17" t="s">
@@ -33732,7 +33797,7 @@
       </c>
       <c r="L13" s="19"/>
       <c r="M13" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N13" s="17" t="s">
         <v>53</v>
@@ -33743,13 +33808,13 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="17" t="s">
@@ -33765,7 +33830,7 @@
       </c>
       <c r="L14" s="19"/>
       <c r="M14" s="17" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="N14" s="17" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Adds dpv:InformationAudit; closes #202
- adds `dpv:InformationAudit` to Organisational Measures in DPV
- adds `dpv:Audit` as the parent concept
- adds `dpv:SecurityAudit` and `dpv:LegalComplianeAudit` as audit types

Co-authored-by: Paul Ryan <71695536+Paul-Ryan76@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/toms.xlsx
+++ b/code/vocab_csv/toms.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="947">
   <si>
     <t>Term</t>
   </si>
@@ -2610,6 +2610,60 @@
   </si>
   <si>
     <t>Supporting entities, including individuals, with negotiating a contract and its terms and conditions</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>An audit is a systematic examination or evaluation of records, processes, or systems towards a specific objective such as to assess accuracy, compliance, effectiveness, or performance</t>
+  </si>
+  <si>
+    <t>SecurityAudit</t>
+  </si>
+  <si>
+    <t>Security Audit</t>
+  </si>
+  <si>
+    <t>An audit that systematically examines the existence and use of security risks and measures within information systems, networks, and security policies to identify vulnerabilities, risks, and gaps</t>
+  </si>
+  <si>
+    <t>dpv:Audit</t>
+  </si>
+  <si>
+    <t>LegalComplianceAudit</t>
+  </si>
+  <si>
+    <t>Legal Compliance Audit</t>
+  </si>
+  <si>
+    <t>An audit that systematically examines the state of legal compliance by reviewing policies and procedures related to obligations and compliance requirements for specific laws and regulations</t>
+  </si>
+  <si>
+    <t>InformationAudit</t>
+  </si>
+  <si>
+    <t>Information Audit</t>
+  </si>
+  <si>
+    <t>An audit that systematically examines the existence and use of information along with its associated resources (e.g. where it is stored) and flows (e.g. where it originates and with whom it is being shared)</t>
+  </si>
+  <si>
+    <t>Paul Ryan, Harshvardhan J. Pandit</t>
+  </si>
+  <si>
+    <t>PersonalDataAudit</t>
+  </si>
+  <si>
+    <t>Personal Data Audit</t>
+  </si>
+  <si>
+    <t>An audit that systematically examines the existence and use of personal data along with its associated resources (e.g. where it is stored) and flows (e.g. where it originates and with whom it is being shared)</t>
+  </si>
+  <si>
+    <t>dpv:InformationAudit</t>
+  </si>
+  <si>
+    <t>This concept is the same as "Data Mapping" and "Data Flow Mapping Exercise" used by the Information Comissioner's Office as "to document the data that flows in, around, and out of information processing systems or services"</t>
   </si>
   <si>
     <t>EnforceTransferControl</t>
@@ -23107,18 +23161,34 @@
       <c r="AF119" s="13"/>
     </row>
     <row r="121">
-      <c r="A121" s="103"/>
-      <c r="B121" s="94"/>
-      <c r="C121" s="104"/>
+      <c r="A121" s="86" t="s">
+        <v>726</v>
+      </c>
+      <c r="B121" s="86" t="s">
+        <v>726</v>
+      </c>
+      <c r="C121" s="81" t="s">
+        <v>727</v>
+      </c>
       <c r="D121" s="86"/>
+      <c r="E121" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="F121" s="73"/>
       <c r="G121" s="94"/>
       <c r="H121" s="73"/>
       <c r="I121" s="73"/>
       <c r="J121" s="94"/>
-      <c r="K121" s="73"/>
+      <c r="K121" s="82">
+        <v>45643.0</v>
+      </c>
       <c r="L121" s="73"/>
-      <c r="N121" s="73"/>
+      <c r="M121" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N121" s="71" t="s">
+        <v>53</v>
+      </c>
       <c r="O121" s="73"/>
       <c r="P121" s="73"/>
       <c r="Q121" s="73"/>
@@ -23139,30 +23209,36 @@
       <c r="AF121" s="73"/>
     </row>
     <row r="122">
-      <c r="A122" s="73" t="s">
-        <v>726</v>
-      </c>
-      <c r="B122" s="73" t="s">
-        <v>727</v>
-      </c>
-      <c r="C122" s="99" t="s">
+      <c r="A122" s="86" t="s">
         <v>728</v>
       </c>
-      <c r="D122" s="73"/>
+      <c r="B122" s="86" t="s">
+        <v>729</v>
+      </c>
+      <c r="C122" s="81" t="s">
+        <v>730</v>
+      </c>
+      <c r="D122" s="86" t="s">
+        <v>731</v>
+      </c>
       <c r="E122" s="17" t="s">
         <v>58</v>
       </c>
       <c r="F122" s="73"/>
-      <c r="G122" s="73"/>
+      <c r="G122" s="94"/>
       <c r="H122" s="73"/>
       <c r="I122" s="73"/>
-      <c r="J122" s="73"/>
-      <c r="K122" s="73"/>
+      <c r="J122" s="94"/>
+      <c r="K122" s="82">
+        <v>45643.0</v>
+      </c>
       <c r="L122" s="73"/>
       <c r="M122" s="17" t="s">
-        <v>729</v>
-      </c>
-      <c r="N122" s="73"/>
+        <v>20</v>
+      </c>
+      <c r="N122" s="71" t="s">
+        <v>53</v>
+      </c>
       <c r="O122" s="73"/>
       <c r="P122" s="73"/>
       <c r="Q122" s="73"/>
@@ -23179,39 +23255,43 @@
       <c r="AB122" s="73"/>
       <c r="AC122" s="73"/>
       <c r="AD122" s="73"/>
+      <c r="AE122" s="73"/>
+      <c r="AF122" s="73"/>
     </row>
     <row r="123">
-      <c r="A123" s="83" t="s">
-        <v>730</v>
-      </c>
-      <c r="B123" s="89"/>
-      <c r="C123" s="85" t="s">
+      <c r="A123" s="86" t="s">
+        <v>732</v>
+      </c>
+      <c r="B123" s="86" t="s">
+        <v>733</v>
+      </c>
+      <c r="C123" s="81" t="s">
+        <v>734</v>
+      </c>
+      <c r="D123" s="86" t="s">
         <v>731</v>
       </c>
-      <c r="D123" s="113" t="s">
-        <v>51</v>
-      </c>
-      <c r="E123" s="87" t="s">
+      <c r="E123" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F123" s="88"/>
-      <c r="G123" s="88"/>
-      <c r="H123" s="88"/>
-      <c r="I123" s="89"/>
-      <c r="J123" s="89"/>
+      <c r="F123" s="73"/>
+      <c r="G123" s="94"/>
+      <c r="H123" s="73"/>
+      <c r="I123" s="73"/>
+      <c r="J123" s="94"/>
       <c r="K123" s="82">
-        <v>45396.0</v>
-      </c>
-      <c r="L123" s="90"/>
-      <c r="M123" s="71" t="s">
-        <v>729</v>
-      </c>
-      <c r="N123" s="85" t="s">
-        <v>220</v>
-      </c>
-      <c r="O123" s="89"/>
-      <c r="P123" s="88"/>
-      <c r="Q123" s="88"/>
+        <v>45643.0</v>
+      </c>
+      <c r="L123" s="73"/>
+      <c r="M123" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N123" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="O123" s="73"/>
+      <c r="P123" s="73"/>
+      <c r="Q123" s="73"/>
       <c r="R123" s="73"/>
       <c r="S123" s="73"/>
       <c r="T123" s="73"/>
@@ -23229,357 +23309,391 @@
       <c r="AF123" s="73"/>
     </row>
     <row r="124">
-      <c r="B124" s="22"/>
-      <c r="N124" s="114"/>
+      <c r="A124" s="86" t="s">
+        <v>735</v>
+      </c>
+      <c r="B124" s="86" t="s">
+        <v>736</v>
+      </c>
+      <c r="C124" s="81" t="s">
+        <v>737</v>
+      </c>
+      <c r="D124" s="86" t="s">
+        <v>731</v>
+      </c>
+      <c r="E124" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F124" s="73"/>
+      <c r="G124" s="94"/>
+      <c r="H124" s="73"/>
+      <c r="I124" s="73"/>
+      <c r="J124" s="94"/>
+      <c r="K124" s="82">
+        <v>45643.0</v>
+      </c>
+      <c r="L124" s="73"/>
+      <c r="M124" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N124" s="71" t="s">
+        <v>738</v>
+      </c>
+      <c r="O124" s="73"/>
+      <c r="P124" s="73"/>
+      <c r="Q124" s="73"/>
+      <c r="R124" s="73"/>
+      <c r="S124" s="73"/>
+      <c r="T124" s="73"/>
+      <c r="U124" s="73"/>
+      <c r="V124" s="73"/>
+      <c r="W124" s="73"/>
+      <c r="X124" s="73"/>
+      <c r="Y124" s="73"/>
+      <c r="Z124" s="73"/>
+      <c r="AA124" s="73"/>
+      <c r="AB124" s="73"/>
+      <c r="AC124" s="73"/>
+      <c r="AD124" s="73"/>
+      <c r="AE124" s="73"/>
+      <c r="AF124" s="73"/>
     </row>
     <row r="125">
-      <c r="A125" s="17" t="s">
-        <v>732</v>
-      </c>
-      <c r="B125" s="17" t="s">
-        <v>733</v>
-      </c>
-      <c r="C125" s="17" t="s">
-        <v>734</v>
-      </c>
-      <c r="D125" s="19"/>
-      <c r="E125" s="87" t="s">
+      <c r="A125" s="86" t="s">
+        <v>739</v>
+      </c>
+      <c r="B125" s="86" t="s">
+        <v>740</v>
+      </c>
+      <c r="C125" s="81" t="s">
+        <v>741</v>
+      </c>
+      <c r="D125" s="86" t="s">
+        <v>742</v>
+      </c>
+      <c r="E125" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F125" s="19"/>
-      <c r="G125" s="19"/>
-      <c r="H125" s="19"/>
-      <c r="I125" s="19"/>
-      <c r="J125" s="19"/>
-      <c r="K125" s="20">
-        <v>45429.0</v>
-      </c>
-      <c r="L125" s="19"/>
+      <c r="F125" s="73"/>
+      <c r="G125" s="94"/>
+      <c r="H125" s="73"/>
+      <c r="I125" s="71" t="s">
+        <v>743</v>
+      </c>
+      <c r="J125" s="94"/>
+      <c r="K125" s="82">
+        <v>45643.0</v>
+      </c>
+      <c r="L125" s="73"/>
       <c r="M125" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N125" s="17" t="s">
+      <c r="N125" s="71" t="s">
+        <v>738</v>
+      </c>
+      <c r="O125" s="73"/>
+      <c r="P125" s="73"/>
+      <c r="Q125" s="73"/>
+      <c r="R125" s="73"/>
+      <c r="S125" s="73"/>
+      <c r="T125" s="73"/>
+      <c r="U125" s="73"/>
+      <c r="V125" s="73"/>
+      <c r="W125" s="73"/>
+      <c r="X125" s="73"/>
+      <c r="Y125" s="73"/>
+      <c r="Z125" s="73"/>
+      <c r="AA125" s="73"/>
+      <c r="AB125" s="73"/>
+      <c r="AC125" s="73"/>
+      <c r="AD125" s="73"/>
+      <c r="AE125" s="73"/>
+      <c r="AF125" s="73"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="103"/>
+      <c r="B126" s="94"/>
+      <c r="C126" s="104"/>
+      <c r="D126" s="86"/>
+      <c r="F126" s="73"/>
+      <c r="G126" s="94"/>
+      <c r="H126" s="73"/>
+      <c r="I126" s="73"/>
+      <c r="J126" s="94"/>
+      <c r="K126" s="73"/>
+      <c r="L126" s="73"/>
+      <c r="N126" s="73"/>
+      <c r="O126" s="73"/>
+      <c r="P126" s="73"/>
+      <c r="Q126" s="73"/>
+      <c r="R126" s="73"/>
+      <c r="S126" s="73"/>
+      <c r="T126" s="73"/>
+      <c r="U126" s="73"/>
+      <c r="V126" s="73"/>
+      <c r="W126" s="73"/>
+      <c r="X126" s="73"/>
+      <c r="Y126" s="73"/>
+      <c r="Z126" s="73"/>
+      <c r="AA126" s="73"/>
+      <c r="AB126" s="73"/>
+      <c r="AC126" s="73"/>
+      <c r="AD126" s="73"/>
+      <c r="AE126" s="73"/>
+      <c r="AF126" s="73"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="73" t="s">
+        <v>744</v>
+      </c>
+      <c r="B127" s="73" t="s">
+        <v>745</v>
+      </c>
+      <c r="C127" s="99" t="s">
+        <v>746</v>
+      </c>
+      <c r="D127" s="73"/>
+      <c r="E127" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F127" s="73"/>
+      <c r="G127" s="73"/>
+      <c r="H127" s="73"/>
+      <c r="I127" s="73"/>
+      <c r="J127" s="73"/>
+      <c r="K127" s="73"/>
+      <c r="L127" s="73"/>
+      <c r="M127" s="17" t="s">
+        <v>747</v>
+      </c>
+      <c r="N127" s="73"/>
+      <c r="O127" s="73"/>
+      <c r="P127" s="73"/>
+      <c r="Q127" s="73"/>
+      <c r="R127" s="73"/>
+      <c r="S127" s="73"/>
+      <c r="T127" s="73"/>
+      <c r="U127" s="73"/>
+      <c r="V127" s="73"/>
+      <c r="W127" s="73"/>
+      <c r="X127" s="73"/>
+      <c r="Y127" s="73"/>
+      <c r="Z127" s="73"/>
+      <c r="AA127" s="73"/>
+      <c r="AB127" s="73"/>
+      <c r="AC127" s="73"/>
+      <c r="AD127" s="73"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="83" t="s">
+        <v>748</v>
+      </c>
+      <c r="B128" s="89"/>
+      <c r="C128" s="85" t="s">
+        <v>749</v>
+      </c>
+      <c r="D128" s="113" t="s">
+        <v>51</v>
+      </c>
+      <c r="E128" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="F128" s="88"/>
+      <c r="G128" s="88"/>
+      <c r="H128" s="88"/>
+      <c r="I128" s="89"/>
+      <c r="J128" s="89"/>
+      <c r="K128" s="82">
+        <v>45396.0</v>
+      </c>
+      <c r="L128" s="90"/>
+      <c r="M128" s="71" t="s">
+        <v>747</v>
+      </c>
+      <c r="N128" s="85" t="s">
+        <v>220</v>
+      </c>
+      <c r="O128" s="89"/>
+      <c r="P128" s="88"/>
+      <c r="Q128" s="88"/>
+      <c r="R128" s="73"/>
+      <c r="S128" s="73"/>
+      <c r="T128" s="73"/>
+      <c r="U128" s="73"/>
+      <c r="V128" s="73"/>
+      <c r="W128" s="73"/>
+      <c r="X128" s="73"/>
+      <c r="Y128" s="73"/>
+      <c r="Z128" s="73"/>
+      <c r="AA128" s="73"/>
+      <c r="AB128" s="73"/>
+      <c r="AC128" s="73"/>
+      <c r="AD128" s="73"/>
+      <c r="AE128" s="73"/>
+      <c r="AF128" s="73"/>
+    </row>
+    <row r="129">
+      <c r="B129" s="22"/>
+      <c r="N129" s="114"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="17" t="s">
+        <v>750</v>
+      </c>
+      <c r="B130" s="17" t="s">
+        <v>751</v>
+      </c>
+      <c r="C130" s="17" t="s">
+        <v>752</v>
+      </c>
+      <c r="D130" s="19"/>
+      <c r="E130" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="F130" s="19"/>
+      <c r="G130" s="19"/>
+      <c r="H130" s="19"/>
+      <c r="I130" s="19"/>
+      <c r="J130" s="19"/>
+      <c r="K130" s="20">
+        <v>45429.0</v>
+      </c>
+      <c r="L130" s="19"/>
+      <c r="M130" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N130" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="O125" s="19"/>
-      <c r="P125" s="19"/>
-      <c r="Q125" s="19"/>
-      <c r="R125" s="19"/>
-      <c r="S125" s="19"/>
-      <c r="T125" s="19"/>
-      <c r="U125" s="19"/>
-      <c r="V125" s="19"/>
-      <c r="W125" s="19"/>
-      <c r="X125" s="19"/>
-      <c r="Y125" s="19"/>
-      <c r="Z125" s="19"/>
-      <c r="AA125" s="19"/>
-      <c r="AB125" s="19"/>
-      <c r="AC125" s="19"/>
-      <c r="AD125" s="19"/>
-      <c r="AE125" s="19"/>
-      <c r="AF125" s="19"/>
-    </row>
-    <row r="126">
-      <c r="A126" s="17" t="s">
-        <v>735</v>
-      </c>
-      <c r="B126" s="17" t="s">
-        <v>736</v>
-      </c>
-      <c r="C126" s="17" t="s">
-        <v>737</v>
-      </c>
-      <c r="D126" s="17" t="s">
-        <v>738</v>
-      </c>
-      <c r="E126" s="87" t="s">
+      <c r="O130" s="19"/>
+      <c r="P130" s="19"/>
+      <c r="Q130" s="19"/>
+      <c r="R130" s="19"/>
+      <c r="S130" s="19"/>
+      <c r="T130" s="19"/>
+      <c r="U130" s="19"/>
+      <c r="V130" s="19"/>
+      <c r="W130" s="19"/>
+      <c r="X130" s="19"/>
+      <c r="Y130" s="19"/>
+      <c r="Z130" s="19"/>
+      <c r="AA130" s="19"/>
+      <c r="AB130" s="19"/>
+      <c r="AC130" s="19"/>
+      <c r="AD130" s="19"/>
+      <c r="AE130" s="19"/>
+      <c r="AF130" s="19"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="17" t="s">
+        <v>753</v>
+      </c>
+      <c r="B131" s="17" t="s">
+        <v>754</v>
+      </c>
+      <c r="C131" s="17" t="s">
+        <v>755</v>
+      </c>
+      <c r="D131" s="17" t="s">
+        <v>756</v>
+      </c>
+      <c r="E131" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="F126" s="19"/>
-      <c r="G126" s="19"/>
-      <c r="H126" s="19"/>
-      <c r="I126" s="19"/>
-      <c r="J126" s="19"/>
-      <c r="K126" s="20">
+      <c r="F131" s="19"/>
+      <c r="G131" s="19"/>
+      <c r="H131" s="19"/>
+      <c r="I131" s="19"/>
+      <c r="J131" s="19"/>
+      <c r="K131" s="20">
         <v>45429.0</v>
       </c>
-      <c r="L126" s="19"/>
-      <c r="M126" s="17" t="s">
+      <c r="L131" s="19"/>
+      <c r="M131" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N126" s="17" t="s">
+      <c r="N131" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="O126" s="19"/>
-      <c r="P126" s="19"/>
-      <c r="Q126" s="19"/>
-      <c r="R126" s="19"/>
-      <c r="S126" s="19"/>
-      <c r="T126" s="19"/>
-      <c r="U126" s="19"/>
-      <c r="V126" s="19"/>
-      <c r="W126" s="19"/>
-      <c r="X126" s="19"/>
-      <c r="Y126" s="19"/>
-      <c r="Z126" s="19"/>
-      <c r="AA126" s="19"/>
-      <c r="AB126" s="19"/>
-      <c r="AC126" s="19"/>
-      <c r="AD126" s="19"/>
-      <c r="AE126" s="19"/>
-      <c r="AF126" s="19"/>
-    </row>
-    <row r="127">
-      <c r="A127" s="17" t="s">
-        <v>739</v>
-      </c>
-      <c r="B127" s="17" t="s">
-        <v>740</v>
-      </c>
-      <c r="C127" s="17" t="s">
-        <v>741</v>
-      </c>
-      <c r="D127" s="17" t="s">
-        <v>738</v>
-      </c>
-      <c r="E127" s="87" t="s">
+      <c r="O131" s="19"/>
+      <c r="P131" s="19"/>
+      <c r="Q131" s="19"/>
+      <c r="R131" s="19"/>
+      <c r="S131" s="19"/>
+      <c r="T131" s="19"/>
+      <c r="U131" s="19"/>
+      <c r="V131" s="19"/>
+      <c r="W131" s="19"/>
+      <c r="X131" s="19"/>
+      <c r="Y131" s="19"/>
+      <c r="Z131" s="19"/>
+      <c r="AA131" s="19"/>
+      <c r="AB131" s="19"/>
+      <c r="AC131" s="19"/>
+      <c r="AD131" s="19"/>
+      <c r="AE131" s="19"/>
+      <c r="AF131" s="19"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="17" t="s">
+        <v>757</v>
+      </c>
+      <c r="B132" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="C132" s="17" t="s">
+        <v>759</v>
+      </c>
+      <c r="D132" s="17" t="s">
+        <v>756</v>
+      </c>
+      <c r="E132" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="F127" s="19"/>
-      <c r="G127" s="19"/>
-      <c r="H127" s="19"/>
-      <c r="I127" s="19"/>
-      <c r="J127" s="19"/>
-      <c r="K127" s="20">
+      <c r="F132" s="19"/>
+      <c r="G132" s="19"/>
+      <c r="H132" s="19"/>
+      <c r="I132" s="19"/>
+      <c r="J132" s="19"/>
+      <c r="K132" s="20">
         <v>45429.0</v>
       </c>
-      <c r="L127" s="19"/>
-      <c r="M127" s="17" t="s">
+      <c r="L132" s="19"/>
+      <c r="M132" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N127" s="17" t="s">
+      <c r="N132" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="O127" s="19"/>
-      <c r="P127" s="19"/>
-      <c r="Q127" s="19"/>
-      <c r="R127" s="19"/>
-      <c r="S127" s="19"/>
-      <c r="T127" s="19"/>
-      <c r="U127" s="19"/>
-      <c r="V127" s="19"/>
-      <c r="W127" s="19"/>
-      <c r="X127" s="19"/>
-      <c r="Y127" s="19"/>
-      <c r="Z127" s="19"/>
-      <c r="AA127" s="19"/>
-      <c r="AB127" s="19"/>
-      <c r="AC127" s="19"/>
-      <c r="AD127" s="19"/>
-      <c r="AE127" s="19"/>
-      <c r="AF127" s="19"/>
-    </row>
-    <row r="129">
-      <c r="A129" s="8" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="115" t="s">
-        <v>743</v>
-      </c>
-      <c r="B130" s="73"/>
-      <c r="C130" s="73"/>
-      <c r="D130" s="73"/>
-      <c r="E130" s="73"/>
-      <c r="F130" s="73"/>
-      <c r="G130" s="73"/>
-      <c r="H130" s="73"/>
-      <c r="I130" s="73"/>
-      <c r="J130" s="73"/>
-      <c r="K130" s="76"/>
-      <c r="L130" s="76"/>
-      <c r="M130" s="73"/>
-      <c r="N130" s="73"/>
-      <c r="O130" s="73"/>
-      <c r="P130" s="73"/>
-      <c r="Q130" s="73"/>
-      <c r="R130" s="73"/>
-      <c r="S130" s="73"/>
-      <c r="T130" s="73"/>
-      <c r="U130" s="73"/>
-      <c r="V130" s="73"/>
-      <c r="W130" s="73"/>
-      <c r="X130" s="73"/>
-      <c r="Y130" s="73"/>
-      <c r="Z130" s="73"/>
-      <c r="AA130" s="73"/>
-      <c r="AB130" s="73"/>
-      <c r="AC130" s="73"/>
-      <c r="AD130" s="73"/>
-    </row>
-    <row r="131">
-      <c r="A131" s="73" t="s">
-        <v>425</v>
-      </c>
-      <c r="B131" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="C131" s="73" t="s">
-        <v>745</v>
-      </c>
-      <c r="D131" s="73"/>
-      <c r="E131" s="73"/>
-      <c r="F131" s="73"/>
-      <c r="G131" s="73"/>
-      <c r="H131" s="73"/>
-      <c r="I131" s="73"/>
-      <c r="J131" s="73"/>
-      <c r="K131" s="76"/>
-      <c r="L131" s="76"/>
-      <c r="M131" s="73"/>
-      <c r="N131" s="73"/>
-      <c r="O131" s="73"/>
-      <c r="P131" s="73"/>
-      <c r="Q131" s="73"/>
-      <c r="R131" s="73"/>
-      <c r="S131" s="73"/>
-      <c r="T131" s="73"/>
-      <c r="U131" s="73"/>
-      <c r="V131" s="73"/>
-      <c r="W131" s="73"/>
-      <c r="X131" s="73"/>
-      <c r="Y131" s="73"/>
-      <c r="Z131" s="73"/>
-      <c r="AA131" s="73"/>
-      <c r="AB131" s="73"/>
-      <c r="AC131" s="73"/>
-      <c r="AD131" s="73"/>
-    </row>
-    <row r="132">
-      <c r="A132" s="73" t="s">
-        <v>746</v>
-      </c>
-      <c r="B132" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="C132" s="73" t="s">
-        <v>747</v>
-      </c>
-      <c r="D132" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="E132" s="73"/>
-      <c r="F132" s="73"/>
-      <c r="G132" s="73"/>
-      <c r="H132" s="73"/>
-      <c r="I132" s="73"/>
-      <c r="J132" s="73"/>
-      <c r="K132" s="76"/>
-      <c r="L132" s="76"/>
-      <c r="M132" s="73"/>
-      <c r="N132" s="73"/>
-      <c r="O132" s="73"/>
-      <c r="P132" s="73"/>
-      <c r="Q132" s="73"/>
-      <c r="R132" s="73"/>
-      <c r="S132" s="73"/>
-      <c r="T132" s="73"/>
-      <c r="U132" s="73"/>
-      <c r="V132" s="73"/>
-      <c r="W132" s="73"/>
-      <c r="X132" s="73"/>
-      <c r="Y132" s="73"/>
-      <c r="Z132" s="73"/>
-      <c r="AA132" s="73"/>
-      <c r="AB132" s="73"/>
-      <c r="AC132" s="73"/>
-      <c r="AD132" s="73"/>
-    </row>
-    <row r="133">
-      <c r="A133" s="73" t="s">
-        <v>748</v>
-      </c>
-      <c r="B133" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="C133" s="73" t="s">
-        <v>749</v>
-      </c>
-      <c r="D133" s="73"/>
-      <c r="E133" s="73"/>
-      <c r="F133" s="73"/>
-      <c r="G133" s="73"/>
-      <c r="H133" s="73"/>
-      <c r="I133" s="73"/>
-      <c r="J133" s="73"/>
-      <c r="K133" s="76"/>
-      <c r="L133" s="76"/>
-      <c r="M133" s="73"/>
-      <c r="N133" s="73"/>
-      <c r="O133" s="73"/>
-      <c r="P133" s="73"/>
-      <c r="Q133" s="73"/>
-      <c r="R133" s="73"/>
-      <c r="S133" s="73"/>
-      <c r="T133" s="73"/>
-      <c r="U133" s="73"/>
-      <c r="V133" s="73"/>
-      <c r="W133" s="73"/>
-      <c r="X133" s="73"/>
-      <c r="Y133" s="73"/>
-      <c r="Z133" s="73"/>
-      <c r="AA133" s="73"/>
-      <c r="AB133" s="73"/>
-      <c r="AC133" s="73"/>
-      <c r="AD133" s="73"/>
+      <c r="O132" s="19"/>
+      <c r="P132" s="19"/>
+      <c r="Q132" s="19"/>
+      <c r="R132" s="19"/>
+      <c r="S132" s="19"/>
+      <c r="T132" s="19"/>
+      <c r="U132" s="19"/>
+      <c r="V132" s="19"/>
+      <c r="W132" s="19"/>
+      <c r="X132" s="19"/>
+      <c r="Y132" s="19"/>
+      <c r="Z132" s="19"/>
+      <c r="AA132" s="19"/>
+      <c r="AB132" s="19"/>
+      <c r="AC132" s="19"/>
+      <c r="AD132" s="19"/>
+      <c r="AE132" s="19"/>
+      <c r="AF132" s="19"/>
     </row>
     <row r="134">
-      <c r="A134" s="73" t="s">
-        <v>750</v>
-      </c>
-      <c r="B134" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="C134" s="73" t="s">
-        <v>751</v>
-      </c>
-      <c r="D134" s="73"/>
-      <c r="E134" s="73"/>
-      <c r="F134" s="73"/>
-      <c r="G134" s="73"/>
-      <c r="H134" s="73"/>
-      <c r="I134" s="73"/>
-      <c r="J134" s="73"/>
-      <c r="K134" s="76"/>
-      <c r="L134" s="76"/>
-      <c r="M134" s="73"/>
-      <c r="N134" s="73"/>
-      <c r="O134" s="73"/>
-      <c r="P134" s="73"/>
-      <c r="Q134" s="73"/>
-      <c r="R134" s="73"/>
-      <c r="S134" s="73"/>
-      <c r="T134" s="73"/>
-      <c r="U134" s="73"/>
-      <c r="V134" s="73"/>
-      <c r="W134" s="73"/>
-      <c r="X134" s="73"/>
-      <c r="Y134" s="73"/>
-      <c r="Z134" s="73"/>
-      <c r="AA134" s="73"/>
-      <c r="AB134" s="73"/>
-      <c r="AC134" s="73"/>
-      <c r="AD134" s="73"/>
+      <c r="A134" s="8" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="135">
-      <c r="A135" s="73" t="s">
-        <v>752</v>
-      </c>
-      <c r="B135" s="73" t="s">
-        <v>744</v>
-      </c>
+      <c r="A135" s="115" t="s">
+        <v>761</v>
+      </c>
+      <c r="B135" s="73"/>
       <c r="C135" s="73"/>
       <c r="D135" s="73"/>
       <c r="E135" s="73"/>
@@ -23611,12 +23725,14 @@
     </row>
     <row r="136">
       <c r="A136" s="73" t="s">
-        <v>753</v>
+        <v>425</v>
       </c>
       <c r="B136" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="C136" s="73"/>
+        <v>762</v>
+      </c>
+      <c r="C136" s="73" t="s">
+        <v>763</v>
+      </c>
       <c r="D136" s="73"/>
       <c r="E136" s="73"/>
       <c r="F136" s="73"/>
@@ -23647,13 +23763,17 @@
     </row>
     <row r="137">
       <c r="A137" s="73" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="B137" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="C137" s="73"/>
-      <c r="D137" s="73"/>
+        <v>762</v>
+      </c>
+      <c r="C137" s="73" t="s">
+        <v>765</v>
+      </c>
+      <c r="D137" s="73" t="s">
+        <v>762</v>
+      </c>
       <c r="E137" s="73"/>
       <c r="F137" s="73"/>
       <c r="G137" s="73"/>
@@ -23683,12 +23803,14 @@
     </row>
     <row r="138">
       <c r="A138" s="73" t="s">
-        <v>755</v>
+        <v>766</v>
       </c>
       <c r="B138" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="C138" s="73"/>
+        <v>762</v>
+      </c>
+      <c r="C138" s="73" t="s">
+        <v>767</v>
+      </c>
       <c r="D138" s="73"/>
       <c r="E138" s="73"/>
       <c r="F138" s="73"/>
@@ -23719,12 +23841,14 @@
     </row>
     <row r="139">
       <c r="A139" s="73" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="B139" s="73" t="s">
-        <v>744</v>
-      </c>
-      <c r="C139" s="73"/>
+        <v>762</v>
+      </c>
+      <c r="C139" s="73" t="s">
+        <v>769</v>
+      </c>
       <c r="D139" s="73"/>
       <c r="E139" s="73"/>
       <c r="F139" s="73"/>
@@ -23755,10 +23879,10 @@
     </row>
     <row r="140">
       <c r="A140" s="73" t="s">
-        <v>757</v>
+        <v>770</v>
       </c>
       <c r="B140" s="73" t="s">
-        <v>744</v>
+        <v>762</v>
       </c>
       <c r="C140" s="73"/>
       <c r="D140" s="73"/>
@@ -23791,10 +23915,10 @@
     </row>
     <row r="141">
       <c r="A141" s="73" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="B141" s="73" t="s">
-        <v>744</v>
+        <v>762</v>
       </c>
       <c r="C141" s="73"/>
       <c r="D141" s="73"/>
@@ -23827,10 +23951,10 @@
     </row>
     <row r="142">
       <c r="A142" s="73" t="s">
-        <v>759</v>
+        <v>772</v>
       </c>
       <c r="B142" s="73" t="s">
-        <v>744</v>
+        <v>762</v>
       </c>
       <c r="C142" s="73"/>
       <c r="D142" s="73"/>
@@ -23863,10 +23987,10 @@
     </row>
     <row r="143">
       <c r="A143" s="73" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="B143" s="73" t="s">
-        <v>744</v>
+        <v>762</v>
       </c>
       <c r="C143" s="73"/>
       <c r="D143" s="73"/>
@@ -23899,10 +24023,10 @@
     </row>
     <row r="144">
       <c r="A144" s="73" t="s">
-        <v>761</v>
+        <v>774</v>
       </c>
       <c r="B144" s="73" t="s">
-        <v>744</v>
+        <v>762</v>
       </c>
       <c r="C144" s="73"/>
       <c r="D144" s="73"/>
@@ -23935,10 +24059,10 @@
     </row>
     <row r="145">
       <c r="A145" s="73" t="s">
+        <v>775</v>
+      </c>
+      <c r="B145" s="73" t="s">
         <v>762</v>
-      </c>
-      <c r="B145" s="73" t="s">
-        <v>763</v>
       </c>
       <c r="C145" s="73"/>
       <c r="D145" s="73"/>
@@ -23971,10 +24095,10 @@
     </row>
     <row r="146">
       <c r="A146" s="73" t="s">
-        <v>36</v>
+        <v>776</v>
       </c>
       <c r="B146" s="73" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C146" s="73"/>
       <c r="D146" s="73"/>
@@ -24007,9 +24131,11 @@
     </row>
     <row r="147">
       <c r="A147" s="73" t="s">
-        <v>765</v>
-      </c>
-      <c r="B147" s="73"/>
+        <v>777</v>
+      </c>
+      <c r="B147" s="73" t="s">
+        <v>762</v>
+      </c>
       <c r="C147" s="73"/>
       <c r="D147" s="73"/>
       <c r="E147" s="73"/>
@@ -24041,9 +24167,11 @@
     </row>
     <row r="148">
       <c r="A148" s="73" t="s">
-        <v>766</v>
-      </c>
-      <c r="B148" s="73"/>
+        <v>778</v>
+      </c>
+      <c r="B148" s="73" t="s">
+        <v>762</v>
+      </c>
       <c r="C148" s="73"/>
       <c r="D148" s="73"/>
       <c r="E148" s="73"/>
@@ -24075,9 +24203,11 @@
     </row>
     <row r="149">
       <c r="A149" s="73" t="s">
-        <v>767</v>
-      </c>
-      <c r="B149" s="73"/>
+        <v>779</v>
+      </c>
+      <c r="B149" s="73" t="s">
+        <v>762</v>
+      </c>
       <c r="C149" s="73"/>
       <c r="D149" s="73"/>
       <c r="E149" s="73"/>
@@ -24109,9 +24239,11 @@
     </row>
     <row r="150">
       <c r="A150" s="73" t="s">
-        <v>768</v>
-      </c>
-      <c r="B150" s="73"/>
+        <v>780</v>
+      </c>
+      <c r="B150" s="73" t="s">
+        <v>781</v>
+      </c>
       <c r="C150" s="73"/>
       <c r="D150" s="73"/>
       <c r="E150" s="73"/>
@@ -24143,9 +24275,11 @@
     </row>
     <row r="151">
       <c r="A151" s="73" t="s">
-        <v>769</v>
-      </c>
-      <c r="B151" s="73"/>
+        <v>36</v>
+      </c>
+      <c r="B151" s="73" t="s">
+        <v>782</v>
+      </c>
       <c r="C151" s="73"/>
       <c r="D151" s="73"/>
       <c r="E151" s="73"/>
@@ -24176,7 +24310,9 @@
       <c r="AD151" s="73"/>
     </row>
     <row r="152">
-      <c r="A152" s="73"/>
+      <c r="A152" s="73" t="s">
+        <v>783</v>
+      </c>
       <c r="B152" s="73"/>
       <c r="C152" s="73"/>
       <c r="D152" s="73"/>
@@ -24209,12 +24345,10 @@
     </row>
     <row r="153">
       <c r="A153" s="73" t="s">
-        <v>770</v>
+        <v>784</v>
       </c>
       <c r="B153" s="73"/>
-      <c r="C153" s="73" t="s">
-        <v>771</v>
-      </c>
+      <c r="C153" s="73"/>
       <c r="D153" s="73"/>
       <c r="E153" s="73"/>
       <c r="F153" s="73"/>
@@ -24244,19 +24378,174 @@
       <c r="AD153" s="73"/>
     </row>
     <row r="154">
-      <c r="B154" s="23"/>
+      <c r="A154" s="73" t="s">
+        <v>785</v>
+      </c>
+      <c r="B154" s="73"/>
+      <c r="C154" s="73"/>
+      <c r="D154" s="73"/>
+      <c r="E154" s="73"/>
+      <c r="F154" s="73"/>
+      <c r="G154" s="73"/>
+      <c r="H154" s="73"/>
+      <c r="I154" s="73"/>
+      <c r="J154" s="73"/>
+      <c r="K154" s="76"/>
+      <c r="L154" s="76"/>
+      <c r="M154" s="73"/>
+      <c r="N154" s="73"/>
+      <c r="O154" s="73"/>
+      <c r="P154" s="73"/>
+      <c r="Q154" s="73"/>
+      <c r="R154" s="73"/>
+      <c r="S154" s="73"/>
+      <c r="T154" s="73"/>
+      <c r="U154" s="73"/>
+      <c r="V154" s="73"/>
+      <c r="W154" s="73"/>
+      <c r="X154" s="73"/>
+      <c r="Y154" s="73"/>
+      <c r="Z154" s="73"/>
+      <c r="AA154" s="73"/>
+      <c r="AB154" s="73"/>
+      <c r="AC154" s="73"/>
+      <c r="AD154" s="73"/>
     </row>
     <row r="155">
-      <c r="B155" s="23"/>
+      <c r="A155" s="73" t="s">
+        <v>786</v>
+      </c>
+      <c r="B155" s="73"/>
+      <c r="C155" s="73"/>
+      <c r="D155" s="73"/>
+      <c r="E155" s="73"/>
+      <c r="F155" s="73"/>
+      <c r="G155" s="73"/>
+      <c r="H155" s="73"/>
+      <c r="I155" s="73"/>
+      <c r="J155" s="73"/>
+      <c r="K155" s="76"/>
+      <c r="L155" s="76"/>
+      <c r="M155" s="73"/>
+      <c r="N155" s="73"/>
+      <c r="O155" s="73"/>
+      <c r="P155" s="73"/>
+      <c r="Q155" s="73"/>
+      <c r="R155" s="73"/>
+      <c r="S155" s="73"/>
+      <c r="T155" s="73"/>
+      <c r="U155" s="73"/>
+      <c r="V155" s="73"/>
+      <c r="W155" s="73"/>
+      <c r="X155" s="73"/>
+      <c r="Y155" s="73"/>
+      <c r="Z155" s="73"/>
+      <c r="AA155" s="73"/>
+      <c r="AB155" s="73"/>
+      <c r="AC155" s="73"/>
+      <c r="AD155" s="73"/>
     </row>
     <row r="156">
-      <c r="B156" s="23"/>
+      <c r="A156" s="73" t="s">
+        <v>787</v>
+      </c>
+      <c r="B156" s="73"/>
+      <c r="C156" s="73"/>
+      <c r="D156" s="73"/>
+      <c r="E156" s="73"/>
+      <c r="F156" s="73"/>
+      <c r="G156" s="73"/>
+      <c r="H156" s="73"/>
+      <c r="I156" s="73"/>
+      <c r="J156" s="73"/>
+      <c r="K156" s="76"/>
+      <c r="L156" s="76"/>
+      <c r="M156" s="73"/>
+      <c r="N156" s="73"/>
+      <c r="O156" s="73"/>
+      <c r="P156" s="73"/>
+      <c r="Q156" s="73"/>
+      <c r="R156" s="73"/>
+      <c r="S156" s="73"/>
+      <c r="T156" s="73"/>
+      <c r="U156" s="73"/>
+      <c r="V156" s="73"/>
+      <c r="W156" s="73"/>
+      <c r="X156" s="73"/>
+      <c r="Y156" s="73"/>
+      <c r="Z156" s="73"/>
+      <c r="AA156" s="73"/>
+      <c r="AB156" s="73"/>
+      <c r="AC156" s="73"/>
+      <c r="AD156" s="73"/>
     </row>
     <row r="157">
-      <c r="B157" s="23"/>
+      <c r="A157" s="73"/>
+      <c r="B157" s="73"/>
+      <c r="C157" s="73"/>
+      <c r="D157" s="73"/>
+      <c r="E157" s="73"/>
+      <c r="F157" s="73"/>
+      <c r="G157" s="73"/>
+      <c r="H157" s="73"/>
+      <c r="I157" s="73"/>
+      <c r="J157" s="73"/>
+      <c r="K157" s="76"/>
+      <c r="L157" s="76"/>
+      <c r="M157" s="73"/>
+      <c r="N157" s="73"/>
+      <c r="O157" s="73"/>
+      <c r="P157" s="73"/>
+      <c r="Q157" s="73"/>
+      <c r="R157" s="73"/>
+      <c r="S157" s="73"/>
+      <c r="T157" s="73"/>
+      <c r="U157" s="73"/>
+      <c r="V157" s="73"/>
+      <c r="W157" s="73"/>
+      <c r="X157" s="73"/>
+      <c r="Y157" s="73"/>
+      <c r="Z157" s="73"/>
+      <c r="AA157" s="73"/>
+      <c r="AB157" s="73"/>
+      <c r="AC157" s="73"/>
+      <c r="AD157" s="73"/>
     </row>
     <row r="158">
-      <c r="B158" s="23"/>
+      <c r="A158" s="73" t="s">
+        <v>788</v>
+      </c>
+      <c r="B158" s="73"/>
+      <c r="C158" s="73" t="s">
+        <v>789</v>
+      </c>
+      <c r="D158" s="73"/>
+      <c r="E158" s="73"/>
+      <c r="F158" s="73"/>
+      <c r="G158" s="73"/>
+      <c r="H158" s="73"/>
+      <c r="I158" s="73"/>
+      <c r="J158" s="73"/>
+      <c r="K158" s="76"/>
+      <c r="L158" s="76"/>
+      <c r="M158" s="73"/>
+      <c r="N158" s="73"/>
+      <c r="O158" s="73"/>
+      <c r="P158" s="73"/>
+      <c r="Q158" s="73"/>
+      <c r="R158" s="73"/>
+      <c r="S158" s="73"/>
+      <c r="T158" s="73"/>
+      <c r="U158" s="73"/>
+      <c r="V158" s="73"/>
+      <c r="W158" s="73"/>
+      <c r="X158" s="73"/>
+      <c r="Y158" s="73"/>
+      <c r="Z158" s="73"/>
+      <c r="AA158" s="73"/>
+      <c r="AB158" s="73"/>
+      <c r="AC158" s="73"/>
+      <c r="AD158" s="73"/>
     </row>
     <row r="159">
       <c r="B159" s="23"/>
@@ -26750,6 +27039,21 @@
     </row>
     <row r="989">
       <c r="B989" s="23"/>
+    </row>
+    <row r="990">
+      <c r="B990" s="23"/>
+    </row>
+    <row r="991">
+      <c r="B991" s="23"/>
+    </row>
+    <row r="992">
+      <c r="B992" s="23"/>
+    </row>
+    <row r="993">
+      <c r="B993" s="23"/>
+    </row>
+    <row r="994">
+      <c r="B994" s="23"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AF3">
@@ -26762,17 +27066,17 @@
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:AF219">
+  <conditionalFormatting sqref="A4:AF224">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M4="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Q1 A4:Q222">
+  <conditionalFormatting sqref="A1:Q1 A4:Q227">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M1="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Q1 A4:Q222">
+  <conditionalFormatting sqref="A1:Q1 A4:Q227">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>$M1="changed"</formula>
     </cfRule>
@@ -27232,7 +27536,7 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>772</v>
+        <v>790</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -27241,13 +27545,13 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>773</v>
+        <v>791</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>774</v>
+        <v>792</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>775</v>
+        <v>793</v>
       </c>
       <c r="D10" s="74" t="s">
         <v>74</v>
@@ -27260,7 +27564,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K10" s="82">
         <v>45521.0</v>
@@ -27291,13 +27595,13 @@
     </row>
     <row r="11">
       <c r="A11" s="71" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="B11" s="71" t="s">
-        <v>778</v>
+        <v>796</v>
       </c>
       <c r="C11" s="71" t="s">
-        <v>779</v>
+        <v>797</v>
       </c>
       <c r="D11" s="74" t="s">
         <v>74</v>
@@ -27310,7 +27614,7 @@
       <c r="H11" s="73"/>
       <c r="I11" s="73"/>
       <c r="J11" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K11" s="82">
         <v>45521.0</v>
@@ -27341,13 +27645,13 @@
     </row>
     <row r="12">
       <c r="A12" s="71" t="s">
-        <v>780</v>
+        <v>798</v>
       </c>
       <c r="B12" s="71" t="s">
-        <v>781</v>
+        <v>799</v>
       </c>
       <c r="C12" s="116" t="s">
-        <v>782</v>
+        <v>800</v>
       </c>
       <c r="D12" s="74" t="s">
         <v>74</v>
@@ -27360,7 +27664,7 @@
       <c r="H12" s="73"/>
       <c r="I12" s="73"/>
       <c r="J12" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K12" s="82">
         <v>45521.0</v>
@@ -27391,13 +27695,13 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>783</v>
+        <v>801</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>784</v>
+        <v>802</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>785</v>
+        <v>803</v>
       </c>
       <c r="D13" s="74" t="s">
         <v>74</v>
@@ -27410,7 +27714,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K13" s="82">
         <v>45521.0</v>
@@ -27441,13 +27745,13 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>786</v>
+        <v>804</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>787</v>
+        <v>805</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>788</v>
+        <v>806</v>
       </c>
       <c r="D14" s="74" t="s">
         <v>74</v>
@@ -27460,7 +27764,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
       <c r="J14" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K14" s="82">
         <v>45521.0</v>
@@ -27491,13 +27795,13 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>789</v>
+        <v>807</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>790</v>
+        <v>808</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>791</v>
+        <v>809</v>
       </c>
       <c r="D15" s="74" t="s">
         <v>74</v>
@@ -27510,7 +27814,7 @@
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K15" s="82">
         <v>45521.0</v>
@@ -27541,13 +27845,13 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>792</v>
+        <v>810</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>793</v>
+        <v>811</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>794</v>
+        <v>812</v>
       </c>
       <c r="D16" s="74" t="s">
         <v>74</v>
@@ -27560,7 +27864,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K16" s="82">
         <v>45521.0</v>
@@ -27591,13 +27895,13 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>795</v>
+        <v>813</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>796</v>
+        <v>814</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>797</v>
+        <v>815</v>
       </c>
       <c r="D17" s="74" t="s">
         <v>74</v>
@@ -27610,7 +27914,7 @@
       <c r="H17" s="19"/>
       <c r="I17" s="49"/>
       <c r="J17" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K17" s="82">
         <v>45521.0</v>
@@ -27649,13 +27953,13 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>798</v>
+        <v>816</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>799</v>
+        <v>817</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>800</v>
+        <v>818</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>18</v>
@@ -27668,7 +27972,7 @@
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K19" s="82">
         <v>45521.0</v>
@@ -27699,13 +28003,13 @@
     </row>
     <row r="20">
       <c r="A20" s="17" t="s">
-        <v>801</v>
+        <v>819</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>802</v>
+        <v>820</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>803</v>
+        <v>821</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>18</v>
@@ -27718,7 +28022,7 @@
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
       <c r="J20" s="17" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="K20" s="82">
         <v>45521.0</v>
@@ -27755,13 +28059,13 @@
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>804</v>
+        <v>822</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>805</v>
+        <v>823</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>806</v>
+        <v>824</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>74</v>
@@ -27805,17 +28109,17 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>807</v>
+        <v>825</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>808</v>
+        <v>826</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>809</v>
+        <v>827</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="17" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -27853,17 +28157,17 @@
     </row>
     <row r="24">
       <c r="A24" s="17" t="s">
-        <v>811</v>
+        <v>829</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>812</v>
+        <v>830</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>813</v>
+        <v>831</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="17" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -27901,17 +28205,17 @@
     </row>
     <row r="25">
       <c r="A25" s="17" t="s">
-        <v>814</v>
+        <v>832</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>815</v>
+        <v>833</v>
       </c>
       <c r="C25" s="79" t="s">
-        <v>816</v>
+        <v>834</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="17" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -27949,17 +28253,17 @@
     </row>
     <row r="26">
       <c r="A26" s="17" t="s">
-        <v>817</v>
+        <v>835</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="C26" s="79" t="s">
-        <v>819</v>
+        <v>837</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="17" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -27997,17 +28301,17 @@
     </row>
     <row r="27">
       <c r="A27" s="17" t="s">
-        <v>820</v>
+        <v>838</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>821</v>
+        <v>839</v>
       </c>
       <c r="C27" s="79" t="s">
-        <v>822</v>
+        <v>840</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="17" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
@@ -28045,17 +28349,17 @@
     </row>
     <row r="28">
       <c r="A28" s="17" t="s">
-        <v>823</v>
+        <v>841</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>824</v>
+        <v>842</v>
       </c>
       <c r="C28" s="79" t="s">
-        <v>825</v>
+        <v>843</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="17" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
@@ -28093,17 +28397,17 @@
     </row>
     <row r="29">
       <c r="A29" s="17" t="s">
-        <v>826</v>
+        <v>844</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>827</v>
+        <v>845</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>828</v>
+        <v>846</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="17" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
@@ -32368,19 +32672,19 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>829</v>
+        <v>847</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>830</v>
+        <v>848</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>831</v>
+        <v>849</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>832</v>
+        <v>850</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>833</v>
+        <v>851</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
@@ -32412,19 +32716,19 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>834</v>
+        <v>852</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>835</v>
+        <v>853</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>836</v>
+        <v>854</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>837</v>
+        <v>855</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
@@ -32456,19 +32760,19 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>838</v>
+        <v>856</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>839</v>
+        <v>857</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>840</v>
+        <v>858</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>74</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -35492,13 +35796,13 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>841</v>
+        <v>859</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>842</v>
+        <v>860</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>843</v>
+        <v>861</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>81</v>
@@ -35511,7 +35815,7 @@
         <v>45531.0</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>844</v>
+        <v>862</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>28</v>
@@ -35522,13 +35826,13 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>845</v>
+        <v>863</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>846</v>
+        <v>864</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>847</v>
+        <v>865</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>81</v>
@@ -35541,7 +35845,7 @@
         <v>45531.0</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>844</v>
+        <v>862</v>
       </c>
       <c r="N3" s="17" t="s">
         <v>28</v>
@@ -35552,16 +35856,16 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>848</v>
+        <v>866</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>849</v>
+        <v>867</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>850</v>
+        <v>868</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>851</v>
+        <v>869</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>81</v>
@@ -35599,16 +35903,16 @@
     </row>
     <row r="5">
       <c r="A5" s="126" t="s">
-        <v>852</v>
+        <v>870</v>
       </c>
       <c r="B5" s="127" t="s">
-        <v>853</v>
+        <v>871</v>
       </c>
       <c r="C5" s="128" t="s">
-        <v>854</v>
+        <v>872</v>
       </c>
       <c r="D5" s="128" t="s">
-        <v>855</v>
+        <v>873</v>
       </c>
       <c r="E5" s="128" t="s">
         <v>81</v>
@@ -35617,7 +35921,7 @@
       <c r="G5" s="129"/>
       <c r="H5" s="129"/>
       <c r="I5" s="128" t="s">
-        <v>856</v>
+        <v>874</v>
       </c>
       <c r="J5" s="129"/>
       <c r="K5" s="130">
@@ -35626,7 +35930,7 @@
       <c r="L5" s="129"/>
       <c r="M5" s="128"/>
       <c r="N5" s="128" t="s">
-        <v>857</v>
+        <v>875</v>
       </c>
       <c r="O5" s="131" t="s">
         <v>63</v>
@@ -35650,16 +35954,16 @@
     </row>
     <row r="6">
       <c r="A6" s="128" t="s">
-        <v>858</v>
+        <v>876</v>
       </c>
       <c r="B6" s="127" t="s">
-        <v>859</v>
+        <v>877</v>
       </c>
       <c r="C6" s="128" t="s">
-        <v>860</v>
+        <v>878</v>
       </c>
       <c r="D6" s="128" t="s">
-        <v>861</v>
+        <v>879</v>
       </c>
       <c r="E6" s="128" t="s">
         <v>81</v>
@@ -35675,7 +35979,7 @@
       <c r="L6" s="129"/>
       <c r="M6" s="128"/>
       <c r="N6" s="128" t="s">
-        <v>857</v>
+        <v>875</v>
       </c>
       <c r="O6" s="131" t="s">
         <v>63</v>
@@ -35699,16 +36003,16 @@
     </row>
     <row r="7">
       <c r="A7" s="128" t="s">
-        <v>862</v>
+        <v>880</v>
       </c>
       <c r="B7" s="127" t="s">
-        <v>863</v>
+        <v>881</v>
       </c>
       <c r="C7" s="128" t="s">
-        <v>864</v>
+        <v>882</v>
       </c>
       <c r="D7" s="128" t="s">
-        <v>861</v>
+        <v>879</v>
       </c>
       <c r="E7" s="128" t="s">
         <v>81</v>
@@ -35724,7 +36028,7 @@
       <c r="L7" s="129"/>
       <c r="M7" s="128"/>
       <c r="N7" s="128" t="s">
-        <v>857</v>
+        <v>875</v>
       </c>
       <c r="O7" s="131" t="s">
         <v>63</v>
@@ -35748,16 +36052,16 @@
     </row>
     <row r="8">
       <c r="A8" s="128" t="s">
-        <v>865</v>
+        <v>883</v>
       </c>
       <c r="B8" s="127" t="s">
-        <v>866</v>
+        <v>884</v>
       </c>
       <c r="C8" s="128" t="s">
-        <v>867</v>
+        <v>885</v>
       </c>
       <c r="D8" s="128" t="s">
-        <v>861</v>
+        <v>879</v>
       </c>
       <c r="E8" s="128" t="s">
         <v>81</v>
@@ -35773,7 +36077,7 @@
       <c r="L8" s="129"/>
       <c r="M8" s="128"/>
       <c r="N8" s="128" t="s">
-        <v>857</v>
+        <v>875</v>
       </c>
       <c r="O8" s="131" t="s">
         <v>63</v>
@@ -35797,16 +36101,16 @@
     </row>
     <row r="9">
       <c r="A9" s="128" t="s">
-        <v>868</v>
+        <v>886</v>
       </c>
       <c r="B9" s="128" t="s">
-        <v>869</v>
+        <v>887</v>
       </c>
       <c r="C9" s="128" t="s">
-        <v>870</v>
+        <v>888</v>
       </c>
       <c r="D9" s="128" t="s">
-        <v>861</v>
+        <v>879</v>
       </c>
       <c r="E9" s="128" t="s">
         <v>81</v>
@@ -35879,16 +36183,16 @@
     </row>
     <row r="11">
       <c r="A11" s="133" t="s">
-        <v>871</v>
+        <v>889</v>
       </c>
       <c r="B11" s="86" t="s">
-        <v>872</v>
+        <v>890</v>
       </c>
       <c r="C11" s="81" t="s">
+        <v>891</v>
+      </c>
+      <c r="D11" s="86" t="s">
         <v>873</v>
-      </c>
-      <c r="D11" s="86" t="s">
-        <v>855</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>81</v>
@@ -35898,7 +36202,7 @@
       <c r="H11" s="73"/>
       <c r="I11" s="73"/>
       <c r="J11" s="94" t="s">
-        <v>874</v>
+        <v>892</v>
       </c>
       <c r="K11" s="20">
         <v>44601.0</v>
@@ -35930,16 +36234,16 @@
     </row>
     <row r="12">
       <c r="A12" s="134" t="s">
-        <v>875</v>
+        <v>893</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>876</v>
+        <v>894</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>877</v>
+        <v>895</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>855</v>
+        <v>873</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>81</v>
@@ -35979,16 +36283,16 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>878</v>
+        <v>896</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>879</v>
+        <v>897</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>880</v>
+        <v>898</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>855</v>
+        <v>873</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>81</v>
@@ -36035,30 +36339,30 @@
     </row>
     <row r="15">
       <c r="A15" s="135" t="s">
-        <v>881</v>
+        <v>899</v>
       </c>
       <c r="B15" s="136" t="s">
-        <v>881</v>
+        <v>899</v>
       </c>
       <c r="C15" s="137" t="s">
-        <v>882</v>
+        <v>900</v>
       </c>
       <c r="D15" s="138" t="s">
-        <v>851</v>
+        <v>869</v>
       </c>
       <c r="E15" s="128" t="s">
         <v>81</v>
       </c>
       <c r="F15" s="139"/>
       <c r="G15" s="138" t="s">
-        <v>883</v>
+        <v>901</v>
       </c>
       <c r="H15" s="138" t="s">
-        <v>884</v>
+        <v>902</v>
       </c>
       <c r="I15" s="139"/>
       <c r="J15" s="138" t="s">
-        <v>885</v>
+        <v>903</v>
       </c>
       <c r="K15" s="130">
         <v>44601.0</v>
@@ -38794,13 +39098,13 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>886</v>
+        <v>904</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>887</v>
+        <v>905</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>888</v>
+        <v>906</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>113</v>
@@ -38813,7 +39117,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="17" t="s">
-        <v>889</v>
+        <v>907</v>
       </c>
       <c r="K2" s="20">
         <v>44727.0</v>
@@ -38847,13 +39151,13 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>890</v>
+        <v>908</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>891</v>
+        <v>909</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>892</v>
+        <v>910</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="17" t="s">
@@ -38864,7 +39168,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="17" t="s">
-        <v>893</v>
+        <v>911</v>
       </c>
       <c r="K3" s="66">
         <v>45396.0</v>
@@ -38896,13 +39200,13 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>894</v>
+        <v>912</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>895</v>
+        <v>913</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>896</v>
+        <v>914</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="17" t="s">
@@ -38913,7 +39217,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="93"/>
       <c r="J4" s="17" t="s">
-        <v>897</v>
+        <v>915</v>
       </c>
       <c r="K4" s="66">
         <v>45396.0</v>
@@ -38945,13 +39249,13 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>898</v>
+        <v>916</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>899</v>
+        <v>917</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>900</v>
+        <v>918</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="17" t="s">
@@ -38962,7 +39266,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="17" t="s">
-        <v>901</v>
+        <v>919</v>
       </c>
       <c r="K5" s="66">
         <v>45396.0</v>
@@ -38994,13 +39298,13 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>902</v>
+        <v>920</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>903</v>
+        <v>921</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>904</v>
+        <v>922</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="17" t="s">
@@ -39011,7 +39315,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="17" t="s">
-        <v>905</v>
+        <v>923</v>
       </c>
       <c r="K6" s="66">
         <v>45396.0</v>
@@ -39043,13 +39347,13 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>906</v>
+        <v>924</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>907</v>
+        <v>925</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>908</v>
+        <v>926</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="17" t="s">
@@ -39060,7 +39364,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="17" t="s">
-        <v>909</v>
+        <v>927</v>
       </c>
       <c r="K7" s="66">
         <v>45396.0</v>
@@ -39092,13 +39396,13 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>910</v>
+        <v>928</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>911</v>
+        <v>929</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>912</v>
+        <v>930</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="17" t="s">
@@ -39109,7 +39413,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="17" t="s">
-        <v>913</v>
+        <v>931</v>
       </c>
       <c r="K8" s="66">
         <v>45396.0</v>
@@ -39141,13 +39445,13 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>914</v>
+        <v>932</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>915</v>
+        <v>933</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>916</v>
+        <v>934</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="17" t="s">
@@ -39158,7 +39462,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="17" t="s">
-        <v>917</v>
+        <v>935</v>
       </c>
       <c r="K9" s="66">
         <v>45396.0</v>
@@ -39190,13 +39494,13 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>918</v>
+        <v>936</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>919</v>
+        <v>937</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>920</v>
+        <v>938</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="17" t="s">
@@ -39207,7 +39511,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="17" t="s">
-        <v>921</v>
+        <v>939</v>
       </c>
       <c r="K10" s="66">
         <v>45396.0</v>
@@ -39239,13 +39543,13 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>922</v>
+        <v>940</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>924</v>
+        <v>942</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="17" t="s">
@@ -39256,7 +39560,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="17" t="s">
-        <v>925</v>
+        <v>943</v>
       </c>
       <c r="K11" s="66">
         <v>45396.0</v>
@@ -39288,13 +39592,13 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>926</v>
+        <v>944</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>927</v>
+        <v>945</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>928</v>
+        <v>946</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="17" t="s">
@@ -39305,7 +39609,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="17" t="s">
-        <v>925</v>
+        <v>943</v>
       </c>
       <c r="K12" s="66">
         <v>45396.0</v>

</xml_diff>